<commit_message>
Correcting settings page menu
</commit_message>
<xml_diff>
--- a/sberweb/resources/public/templates/CLIENT_WEB.xlsx
+++ b/sberweb/resources/public/templates/CLIENT_WEB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6954" uniqueCount="5145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6978" uniqueCount="5169">
   <si>
     <t>Эмитент</t>
   </si>
@@ -15456,6 +15456,78 @@
   </si>
   <si>
     <t>25/05/2017</t>
+  </si>
+  <si>
+    <t>XS0583616239</t>
+  </si>
+  <si>
+    <t>XS0583616239 Corp</t>
+  </si>
+  <si>
+    <t>BELRUS 8.95 01/26/18</t>
+  </si>
+  <si>
+    <t>CH0336352825</t>
+  </si>
+  <si>
+    <t>YPFDAR 3 ¾ 09/30/19</t>
+  </si>
+  <si>
+    <t>CH0336352825 Corp</t>
+  </si>
+  <si>
+    <t>CH0246199050</t>
+  </si>
+  <si>
+    <t>KTZKZ 3.638 06/20/22</t>
+  </si>
+  <si>
+    <t>CH0246199050 Corp</t>
+  </si>
+  <si>
+    <t>US92189F1066</t>
+  </si>
+  <si>
+    <t>GDX US Equity</t>
+  </si>
+  <si>
+    <t>VANECK VECTORS GOLD MINERS E</t>
+  </si>
+  <si>
+    <t>XS0923110232</t>
+  </si>
+  <si>
+    <t>XS0923110232 Corp</t>
+  </si>
+  <si>
+    <t>NMOSRM 7 ¼ 04/25/18</t>
+  </si>
+  <si>
+    <t>XS1085735899</t>
+  </si>
+  <si>
+    <t>XS1085735899 Corp</t>
+  </si>
+  <si>
+    <t>PORTUG 5 ⅛ 10/15/24</t>
+  </si>
+  <si>
+    <t>XS1223394914</t>
+  </si>
+  <si>
+    <t>XS1223394914 Corp</t>
+  </si>
+  <si>
+    <t>TCZIRA 4 ¾ 04/29/21</t>
+  </si>
+  <si>
+    <t>US71647NAP42</t>
+  </si>
+  <si>
+    <t>US71647NAP42 Corp</t>
+  </si>
+  <si>
+    <t>PETBRA 8 ⅜ 05/23/21</t>
   </si>
 </sst>
 </file>
@@ -16621,11 +16693,11 @@
   </sheetPr>
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight" activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16874,7 +16946,7 @@
         <v>4666</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" ref="D9:D23" si="0">R9/$R$55</f>
+        <f t="shared" ref="D9:D18" si="0">R9/$R$55</f>
         <v>1.9360789804087713E-2</v>
       </c>
       <c r="E9" s="36">
@@ -22366,101 +22438,6 @@
           <xm:sqref>N34:N38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="250" id="{EF154165-A510-48D6-8441-6E52AFB69160}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>3.5</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K53 K32:K33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="191" id="{114ECFA3-0821-47BE-B7AB-089367875297}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>3.5</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="173" id="{9C82F187-496F-4ACE-BA8C-CD06B1B5CA98}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>3.5</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K9:K31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="75" id="{A6BBD403-352E-48A7-80C6-F5EAACA8076B}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>3.5</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K51:K52 K34:K42</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="57" id="{A6E7F667-E3CA-4B6B-822E-484CF02F32A1}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>3.5</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
-              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K43:K50</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8EFD676A-87DE-4793-A389-333D66B9DA7A}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
@@ -22604,6 +22581,101 @@
           <xm:sqref>J19:J23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="250" id="{EF154165-A510-48D6-8441-6E52AFB69160}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K53 K32:K33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="191" id="{114ECFA3-0821-47BE-B7AB-089367875297}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="173" id="{9C82F187-496F-4ACE-BA8C-CD06B1B5CA98}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K9:K31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="75" id="{A6BBD403-352E-48A7-80C6-F5EAACA8076B}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K51:K52 K34:K42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="57" id="{A6E7F667-E3CA-4B6B-822E-484CF02F32A1}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>3.5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K43:K50</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A70E0C30-2B1F-4119-859A-02C77EEA2754}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
@@ -46112,10 +46184,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C161"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47896,7 +47968,96 @@
         <v>4997</v>
       </c>
     </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>5145</v>
+      </c>
+      <c r="B162" t="s">
+        <v>5146</v>
+      </c>
+      <c r="C162" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>5148</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5150</v>
+      </c>
+      <c r="C163" t="s">
+        <v>5149</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>5151</v>
+      </c>
+      <c r="B164" t="s">
+        <v>5153</v>
+      </c>
+      <c r="C164" t="s">
+        <v>5152</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>5154</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5155</v>
+      </c>
+      <c r="C165" t="s">
+        <v>5156</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>5157</v>
+      </c>
+      <c r="B166" t="s">
+        <v>5158</v>
+      </c>
+      <c r="C166" t="s">
+        <v>5159</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>5160</v>
+      </c>
+      <c r="B167" t="s">
+        <v>5161</v>
+      </c>
+      <c r="C167" t="s">
+        <v>5162</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>5163</v>
+      </c>
+      <c r="B168" t="s">
+        <v>5164</v>
+      </c>
+      <c r="C168" t="s">
+        <v>5165</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>5166</v>
+      </c>
+      <c r="B169" t="s">
+        <v>5167</v>
+      </c>
+      <c r="C169" t="s">
+        <v>5168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding clojure build profiles settings
</commit_message>
<xml_diff>
--- a/sberweb/resources/public/templates/CLIENT_WEB.xlsx
+++ b/sberweb/resources/public/templates/CLIENT_WEB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Client!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$J$32:$P$44</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7803" uniqueCount="5920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7806" uniqueCount="5922">
   <si>
     <t>Эмитент</t>
   </si>
@@ -17781,6 +17781,12 @@
   </si>
   <si>
     <t>GS 0 01/04/19</t>
+  </si>
+  <si>
+    <t>RUAL RX Equity</t>
+  </si>
+  <si>
+    <t>Стоимость позиции по текущей цене (USD) с НКД</t>
   </si>
 </sst>
 </file>
@@ -18957,13 +18963,13 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W56"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18988,17 +18994,18 @@
     <col min="19" max="19" width="14.140625" style="23" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" style="23" customWidth="1"/>
     <col min="21" max="21" width="13" style="23" customWidth="1"/>
-    <col min="22" max="23" width="12.28515625" style="23" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="23"/>
+    <col min="22" max="22" width="12.5703125" style="23" customWidth="1"/>
+    <col min="23" max="24" width="12.28515625" style="23" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="M1" s="42" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="42"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
@@ -19015,7 +19022,7 @@
       </c>
       <c r="O2" s="49"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
         <v>14</v>
       </c>
@@ -19032,23 +19039,23 @@
         <v>41</v>
       </c>
       <c r="L3" s="50">
-        <f>M3/P55</f>
-        <v>9.6957754848492228E-2</v>
+        <f>M3/P54</f>
+        <v>0.10284394231908525</v>
       </c>
       <c r="M3" s="53">
         <f>P32</f>
         <v>332034.52798289154</v>
       </c>
       <c r="N3" s="52">
-        <f>P53</f>
-        <v>3092493.283142006</v>
+        <f>P52</f>
+        <v>2896493.283142006</v>
       </c>
       <c r="O3" s="51">
-        <f>N3/P55</f>
-        <v>0.90304224515150777</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+        <f>N3/P54</f>
+        <v>0.89715605768091478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
@@ -19070,7 +19077,7 @@
       <c r="N4" s="42"/>
       <c r="O4" s="43"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>18</v>
       </c>
@@ -19101,16 +19108,16 @@
       </c>
       <c r="N5" s="45">
         <f>D3*70%-N3</f>
-        <v>14407506.716857994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+        <v>14603506.716857994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D6" s="47"/>
       <c r="E6" s="47"/>
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
     </row>
-    <row r="7" spans="1:23" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -19172,13 +19179,16 @@
         <v>12</v>
       </c>
       <c r="V7" s="2" t="s">
+        <v>5921</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>4676</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>4675</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -19202,8 +19212,9 @@
       <c r="S8" s="36"/>
       <c r="T8" s="36"/>
       <c r="U8" s="37"/>
-    </row>
-    <row r="9" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V8" s="36"/>
+    </row>
+    <row r="9" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="str">
         <f>IF(LEFT(C9,2) = "RU", VLOOKUP(C9,MICEX!$A:$D,4,FALSE),VLOOKUP(C9,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>MMC Norilsk Nickel PJSC</v>
@@ -19212,7 +19223,7 @@
         <v>5393</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" ref="D9:D13" si="0">R9/$R$55</f>
+        <f>R9/$R$54</f>
         <v>3.0510877060802067E-2</v>
       </c>
       <c r="E9" s="36">
@@ -19248,11 +19259,11 @@
         <v>USD</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" ref="M9:M10" si="1">IF(O9&gt;0,Q9/O9-1,0)</f>
+        <f t="shared" ref="M9:M10" si="0">IF(O9&gt;0,Q9/O9-1,0)</f>
         <v>0.10608084636118886</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" ref="N9:N10" si="2">IF(P9&gt;0,R9/P9-1,0)</f>
+        <f t="shared" ref="N9:N10" si="1">IF(P9&gt;0,R9/P9-1,0)</f>
         <v>5.8022922636103091E-2</v>
       </c>
       <c r="O9" s="36">
@@ -19276,23 +19287,27 @@
         <v>600931.05287999939</v>
       </c>
       <c r="T9" s="36">
-        <f t="shared" ref="T9:T13" si="3">R9-P9</f>
+        <f t="shared" ref="T9:T13" si="2">R9-P9</f>
         <v>5799.5999999999913</v>
       </c>
       <c r="U9" s="37">
         <f>VLOOKUP(C9,Data!$B:$P,14,FALSE)</f>
         <v>11.013184187445791</v>
       </c>
-      <c r="V9" s="58" t="str">
-        <f>IF(VLOOKUP(C9,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C9,Data!$B:$P,15,FALSE))</f>
-        <v>22/06/2017</v>
+      <c r="V9" s="36">
+        <f>VLOOKUP(C9,Data!$B:$P,5,FALSE)</f>
+        <v>105753.2</v>
       </c>
       <c r="W9" s="58" t="str">
         <f>IF(VLOOKUP(C9,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C9,Data!$B:$P,15,FALSE))</f>
         <v>22/06/2017</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X9" s="58" t="str">
+        <f>IF(VLOOKUP(C9,Data!$B:$Q,16,FALSE)=0,"",VLOOKUP(C9,Data!$B:$Q,16,FALSE))</f>
+        <v>17/11/2017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="str">
         <f>IF(LEFT(C10,2) = "RU", VLOOKUP(C10,MICEX!$A:$D,4,FALSE),VLOOKUP(C10,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>Altria Group Inc</v>
@@ -19301,7 +19316,7 @@
         <v>5837</v>
       </c>
       <c r="D10" s="7">
-        <f t="shared" si="0"/>
+        <f>R10/$R$54</f>
         <v>1.4098916535927758E-2</v>
       </c>
       <c r="E10" s="36">
@@ -19309,7 +19324,7 @@
         <v>760</v>
       </c>
       <c r="F10" s="36">
-        <f t="shared" ref="F10" si="4">$J$5-P10</f>
+        <f t="shared" ref="F10" si="3">$J$5-P10</f>
         <v>2450001.804</v>
       </c>
       <c r="G10" s="57">
@@ -19325,7 +19340,7 @@
         <v>72.642860412597656</v>
       </c>
       <c r="J10" s="10">
-        <f t="shared" ref="J10" si="5">IF(I10&gt;0,I10/H10-1,0)</f>
+        <f t="shared" ref="J10" si="4">IF(I10&gt;0,I10/H10-1,0)</f>
         <v>0.12974899553029018</v>
       </c>
       <c r="K10" s="9">
@@ -19337,11 +19352,11 @@
         <v>USD</v>
       </c>
       <c r="M10" s="7">
+        <f t="shared" si="0"/>
+        <v>-4.4109015701254695E-2</v>
+      </c>
+      <c r="N10" s="7">
         <f t="shared" si="1"/>
-        <v>-4.4109015701254695E-2</v>
-      </c>
-      <c r="N10" s="7">
-        <f t="shared" si="2"/>
         <v>-2.2604735578859558E-2</v>
       </c>
       <c r="O10" s="36">
@@ -19361,27 +19376,31 @@
         <v>48868</v>
       </c>
       <c r="S10" s="36">
-        <f t="shared" ref="S10:S13" si="6">Q10-O10</f>
+        <f t="shared" ref="S10:S13" si="5">Q10-O10</f>
         <v>-133605.57825239934</v>
       </c>
       <c r="T10" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-1130.1959999999963</v>
       </c>
       <c r="U10" s="37">
         <f>VLOOKUP(C10,Data!$B:$P,14,FALSE)</f>
         <v>4.1044776119402995</v>
       </c>
-      <c r="V10" s="58" t="str">
-        <f>IF(VLOOKUP(C10,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C10,Data!$B:$P,15,FALSE))</f>
-        <v>13/06/2017</v>
+      <c r="V10" s="36">
+        <f>VLOOKUP(C10,Data!$B:$P,5,FALSE)</f>
+        <v>48868</v>
       </c>
       <c r="W10" s="58" t="str">
         <f>IF(VLOOKUP(C10,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C10,Data!$B:$P,15,FALSE))</f>
         <v>13/06/2017</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X10" s="58" t="str">
+        <f>IF(VLOOKUP(C10,Data!$B:$Q,16,FALSE)=0,"",VLOOKUP(C10,Data!$B:$Q,16,FALSE))</f>
+        <v>24/08/2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="39" t="str">
         <f>IF(LEFT(C11,2) = "RU", VLOOKUP(C11,MICEX!$A:$D,4,FALSE),VLOOKUP(C11,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>Highland Gold Mining Ltd</v>
@@ -19390,7 +19409,7 @@
         <v>4669</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" si="0"/>
+        <f>R11/$R$54</f>
         <v>2.1862026021007133E-2</v>
       </c>
       <c r="E11" s="36">
@@ -19398,7 +19417,7 @@
         <v>42000</v>
       </c>
       <c r="F11" s="36">
-        <f t="shared" ref="F11" si="7">$J$5-P11</f>
+        <f t="shared" ref="F11" si="6">$J$5-P11</f>
         <v>2426675.5397800421</v>
       </c>
       <c r="G11" s="57">
@@ -19414,7 +19433,7 @@
         <v>215</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" ref="J11" si="8">IF(I11&gt;0,I11/H11-1,0)</f>
+        <f t="shared" ref="J11" si="7">IF(I11&gt;0,I11/H11-1,0)</f>
         <v>0.53571428571428581</v>
       </c>
       <c r="K11" s="9">
@@ -19426,11 +19445,11 @@
         <v>GBX</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" ref="M11" si="9">IF(O11&gt;0,Q11/O11-1,0)</f>
+        <f t="shared" ref="M11" si="8">IF(O11&gt;0,Q11/O11-1,0)</f>
         <v>7.2459253380069644E-2</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" ref="N11" si="10">IF(P11&gt;0,R11/P11-1,0)</f>
+        <f t="shared" ref="N11" si="9">IF(P11&gt;0,R11/P11-1,0)</f>
         <v>3.3428318038317917E-2</v>
       </c>
       <c r="O11" s="36">
@@ -19450,27 +19469,31 @@
         <v>75775.57359617883</v>
       </c>
       <c r="S11" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>303335.54999999935</v>
       </c>
       <c r="T11" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2451.1133762207464</v>
       </c>
       <c r="U11" s="37">
         <f>VLOOKUP(C11,Data!$B:$P,14,FALSE)</f>
         <v>7.428571156093053</v>
       </c>
-      <c r="V11" s="58" t="str">
-        <f>IF(VLOOKUP(C11,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C11,Data!$B:$P,15,FALSE))</f>
-        <v>20/04/2017</v>
+      <c r="V11" s="36">
+        <f>VLOOKUP(C11,Data!$B:$P,5,FALSE)</f>
+        <v>75775.57359617883</v>
       </c>
       <c r="W11" s="58" t="str">
         <f>IF(VLOOKUP(C11,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C11,Data!$B:$P,15,FALSE))</f>
         <v>20/04/2017</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X11" s="58" t="str">
+        <f>IF(VLOOKUP(C11,Data!$B:$Q,16,FALSE)=0,"",VLOOKUP(C11,Data!$B:$Q,16,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="39" t="str">
         <f>IF(LEFT(C12,2) = "RU", VLOOKUP(C12,MICEX!$A:$D,4,FALSE),VLOOKUP(C12,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>Polymetal International PLC</v>
@@ -19479,7 +19502,7 @@
         <v>51</v>
       </c>
       <c r="D12" s="7">
-        <f t="shared" si="0"/>
+        <f>R12/$R$54</f>
         <v>1.5114077453630201E-2</v>
       </c>
       <c r="E12" s="36">
@@ -19487,7 +19510,7 @@
         <v>4350</v>
       </c>
       <c r="F12" s="36">
-        <f t="shared" ref="F12:F13" si="11">$J$5-P12</f>
+        <f t="shared" ref="F12:F13" si="10">$J$5-P12</f>
         <v>2450116.2575500002</v>
       </c>
       <c r="G12" s="57">
@@ -19503,7 +19526,7 @@
         <v>954.59637451171875</v>
       </c>
       <c r="J12" s="10">
-        <f t="shared" ref="J12:J13" si="12">IF(I12&gt;0,I12/H12-1,0)</f>
+        <f t="shared" ref="J12:J13" si="11">IF(I12&gt;0,I12/H12-1,0)</f>
         <v>2.1504948648174205E-2</v>
       </c>
       <c r="K12" s="9">
@@ -19515,11 +19538,11 @@
         <v>GBX</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" ref="M12:M13" si="13">IF(O12&gt;0,Q12/O12-1,0)</f>
+        <f t="shared" ref="M12:M13" si="12">IF(O12&gt;0,Q12/O12-1,0)</f>
         <v>4.436291759501465E-2</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" ref="N12:N13" si="14">IF(P12&gt;0,R12/P12-1,0)</f>
+        <f t="shared" ref="N12:N13" si="13">IF(P12&gt;0,R12/P12-1,0)</f>
         <v>5.017443262364063E-2</v>
       </c>
       <c r="O12" s="36">
@@ -19539,27 +19562,31 @@
         <v>52386.630924572572</v>
       </c>
       <c r="S12" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>131846.96934418567</v>
       </c>
       <c r="T12" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2502.8884745725663</v>
       </c>
       <c r="U12" s="37">
         <f>VLOOKUP(C12,Data!$B:$P,14,FALSE)</f>
         <v>5.8089467916595803</v>
       </c>
-      <c r="V12" s="58" t="str">
-        <f>IF(VLOOKUP(C12,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C12,Data!$B:$P,15,FALSE))</f>
-        <v>04/05/2017</v>
+      <c r="V12" s="36">
+        <f>VLOOKUP(C12,Data!$B:$P,5,FALSE)</f>
+        <v>52386.630924572572</v>
       </c>
       <c r="W12" s="58" t="str">
         <f>IF(VLOOKUP(C12,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C12,Data!$B:$P,15,FALSE))</f>
         <v>04/05/2017</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X12" s="58" t="str">
+        <f>IF(VLOOKUP(C12,Data!$B:$Q,16,FALSE)=0,"",VLOOKUP(C12,Data!$B:$Q,16,FALSE))</f>
+        <v>29/08/2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="39" t="str">
         <f>IF(LEFT(C13,2) = "RU", VLOOKUP(C13,MICEX!$A:$D,4,FALSE),VLOOKUP(C13,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>Daimler AG</v>
@@ -19568,7 +19595,7 @@
         <v>5633</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" si="0"/>
+        <f>R13/$R$54</f>
         <v>1.6972428033997643E-2</v>
       </c>
       <c r="E13" s="36">
@@ -19576,7 +19603,7 @@
         <v>830</v>
       </c>
       <c r="F13" s="36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2441125.4706870667</v>
       </c>
       <c r="G13" s="57">
@@ -19592,7 +19619,7 @@
         <v>71.13043212890625</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.17980481222269451</v>
       </c>
       <c r="K13" s="9">
@@ -19604,11 +19631,11 @@
         <v>EUR</v>
       </c>
       <c r="M13" s="7">
+        <f t="shared" si="12"/>
+        <v>-2.5486294793532038E-2</v>
+      </c>
+      <c r="N13" s="7">
         <f t="shared" si="13"/>
-        <v>-2.5486294793532038E-2</v>
-      </c>
-      <c r="N13" s="7">
-        <f t="shared" si="14"/>
         <v>-7.9326325500028716E-4</v>
       </c>
       <c r="O13" s="36">
@@ -19628,27 +19655,31 @@
         <v>58827.826312174046</v>
       </c>
       <c r="S13" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-91155.436949499883</v>
       </c>
       <c r="T13" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-46.703000759385759</v>
       </c>
       <c r="U13" s="37">
         <f>VLOOKUP(C13,Data!$B:$P,14,FALSE)</f>
         <v>5.3906120417979766</v>
       </c>
-      <c r="V13" s="58" t="str">
-        <f>IF(VLOOKUP(C13,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C13,Data!$B:$P,15,FALSE))</f>
-        <v>30/03/2017</v>
+      <c r="V13" s="36">
+        <f>VLOOKUP(C13,Data!$B:$P,5,FALSE)</f>
+        <v>58827.826312174046</v>
       </c>
       <c r="W13" s="58" t="str">
         <f>IF(VLOOKUP(C13,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C13,Data!$B:$P,15,FALSE))</f>
         <v>30/03/2017</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="58" t="str">
+        <f>IF(VLOOKUP(C13,Data!$B:$Q,16,FALSE)=0,"",VLOOKUP(C13,Data!$B:$Q,16,FALSE))</f>
+        <v>07/02/2018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="7"/>
@@ -19669,10 +19700,11 @@
       <c r="S14" s="36"/>
       <c r="T14" s="36"/>
       <c r="U14" s="37"/>
-      <c r="V14" s="58"/>
+      <c r="V14" s="36"/>
       <c r="W14" s="58"/>
-    </row>
-    <row r="15" spans="1:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="58"/>
+    </row>
+    <row r="15" spans="1:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="7"/>
@@ -19693,10 +19725,11 @@
       <c r="S15" s="36"/>
       <c r="T15" s="36"/>
       <c r="U15" s="37"/>
-      <c r="V15" s="58"/>
+      <c r="V15" s="36"/>
       <c r="W15" s="58"/>
-    </row>
-    <row r="16" spans="1:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X15" s="58"/>
+    </row>
+    <row r="16" spans="1:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="7"/>
@@ -19717,10 +19750,11 @@
       <c r="S16" s="36"/>
       <c r="T16" s="36"/>
       <c r="U16" s="37"/>
-      <c r="V16" s="58"/>
+      <c r="V16" s="36"/>
       <c r="W16" s="58"/>
-    </row>
-    <row r="17" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X16" s="58"/>
+    </row>
+    <row r="17" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="7"/>
@@ -19741,10 +19775,11 @@
       <c r="S17" s="36"/>
       <c r="T17" s="36"/>
       <c r="U17" s="37"/>
-      <c r="V17" s="58"/>
+      <c r="V17" s="36"/>
       <c r="W17" s="58"/>
-    </row>
-    <row r="18" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="58"/>
+    </row>
+    <row r="18" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="7"/>
@@ -19765,10 +19800,11 @@
       <c r="S18" s="36"/>
       <c r="T18" s="36"/>
       <c r="U18" s="37"/>
-      <c r="V18" s="58"/>
+      <c r="V18" s="36"/>
       <c r="W18" s="58"/>
-    </row>
-    <row r="19" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X18" s="58"/>
+    </row>
+    <row r="19" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="7"/>
@@ -19789,10 +19825,11 @@
       <c r="S19" s="36"/>
       <c r="T19" s="36"/>
       <c r="U19" s="37"/>
-      <c r="V19" s="58"/>
+      <c r="V19" s="36"/>
       <c r="W19" s="58"/>
-    </row>
-    <row r="20" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X19" s="58"/>
+    </row>
+    <row r="20" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="7"/>
@@ -19813,10 +19850,11 @@
       <c r="S20" s="36"/>
       <c r="T20" s="36"/>
       <c r="U20" s="37"/>
-      <c r="V20" s="58"/>
+      <c r="V20" s="36"/>
       <c r="W20" s="58"/>
-    </row>
-    <row r="21" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="58"/>
+    </row>
+    <row r="21" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="7"/>
@@ -19837,10 +19875,11 @@
       <c r="S21" s="36"/>
       <c r="T21" s="36"/>
       <c r="U21" s="37"/>
-      <c r="V21" s="58"/>
+      <c r="V21" s="36"/>
       <c r="W21" s="58"/>
-    </row>
-    <row r="22" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="58"/>
+    </row>
+    <row r="22" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="7"/>
@@ -19861,10 +19900,11 @@
       <c r="S22" s="36"/>
       <c r="T22" s="36"/>
       <c r="U22" s="37"/>
-      <c r="V22" s="58"/>
+      <c r="V22" s="36"/>
       <c r="W22" s="58"/>
-    </row>
-    <row r="23" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="58"/>
+    </row>
+    <row r="23" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="7"/>
@@ -19885,10 +19925,11 @@
       <c r="S23" s="36"/>
       <c r="T23" s="36"/>
       <c r="U23" s="37"/>
-      <c r="V23" s="58"/>
+      <c r="V23" s="36"/>
       <c r="W23" s="58"/>
-    </row>
-    <row r="24" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="58"/>
+    </row>
+    <row r="24" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="39" t="s">
         <v>4669</v>
@@ -19901,8 +19942,8 @@
       <c r="I24" s="9"/>
       <c r="J24" s="10"/>
       <c r="K24" s="9" t="e">
-        <f>IF(C24="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C24="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L24" s="11"/>
       <c r="M24" s="7"/>
@@ -19914,13 +19955,14 @@
       <c r="S24" s="36"/>
       <c r="T24" s="36"/>
       <c r="U24" s="37"/>
-      <c r="V24" s="59"/>
-      <c r="W24" s="58" t="e">
+      <c r="V24" s="36"/>
+      <c r="W24" s="59"/>
+      <c r="X24" s="58" t="e">
         <f>VLOOKUP(C24,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="39" t="s">
         <v>51</v>
@@ -19933,8 +19975,8 @@
       <c r="I25" s="9"/>
       <c r="J25" s="10"/>
       <c r="K25" s="9" t="e">
-        <f>IF(C25="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C25="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L25" s="11"/>
       <c r="M25" s="7"/>
@@ -19946,13 +19988,14 @@
       <c r="S25" s="36"/>
       <c r="T25" s="36"/>
       <c r="U25" s="37"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="58" t="e">
+      <c r="V25" s="36"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="58" t="e">
         <f>VLOOKUP(C25,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="7"/>
@@ -19963,8 +20006,8 @@
       <c r="I26" s="9"/>
       <c r="J26" s="10"/>
       <c r="K26" s="9" t="e">
-        <f>IF(C26="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C26="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L26" s="11"/>
       <c r="M26" s="7"/>
@@ -19976,13 +20019,14 @@
       <c r="S26" s="36"/>
       <c r="T26" s="36"/>
       <c r="U26" s="37"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="58" t="e">
+      <c r="V26" s="36"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="58" t="e">
         <f>VLOOKUP(C26,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="7"/>
@@ -19993,8 +20037,8 @@
       <c r="I27" s="9"/>
       <c r="J27" s="10"/>
       <c r="K27" s="9" t="e">
-        <f>IF(C27="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C27="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="7"/>
@@ -20006,13 +20050,14 @@
       <c r="S27" s="36"/>
       <c r="T27" s="36"/>
       <c r="U27" s="37"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="58" t="e">
+      <c r="V27" s="36"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="58" t="e">
         <f>VLOOKUP(C27,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="7"/>
@@ -20023,8 +20068,8 @@
       <c r="I28" s="9"/>
       <c r="J28" s="10"/>
       <c r="K28" s="9" t="e">
-        <f>IF(C28="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C28="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="7"/>
@@ -20036,13 +20081,14 @@
       <c r="S28" s="36"/>
       <c r="T28" s="36"/>
       <c r="U28" s="37"/>
-      <c r="V28" s="59"/>
-      <c r="W28" s="58" t="e">
+      <c r="V28" s="36"/>
+      <c r="W28" s="59"/>
+      <c r="X28" s="58" t="e">
         <f>VLOOKUP(C28,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="7"/>
@@ -20053,8 +20099,8 @@
       <c r="I29" s="9"/>
       <c r="J29" s="10"/>
       <c r="K29" s="9" t="e">
-        <f>IF(C29="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C29="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="7"/>
@@ -20066,13 +20112,14 @@
       <c r="S29" s="36"/>
       <c r="T29" s="36"/>
       <c r="U29" s="37"/>
-      <c r="V29" s="59"/>
-      <c r="W29" s="58" t="e">
+      <c r="V29" s="36"/>
+      <c r="W29" s="59"/>
+      <c r="X29" s="58" t="e">
         <f>VLOOKUP(C29,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="7"/>
@@ -20083,8 +20130,8 @@
       <c r="I30" s="9"/>
       <c r="J30" s="10"/>
       <c r="K30" s="9" t="e">
-        <f>IF(C30="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C30="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="7"/>
@@ -20096,13 +20143,14 @@
       <c r="S30" s="36"/>
       <c r="T30" s="36"/>
       <c r="U30" s="37"/>
-      <c r="V30" s="59"/>
-      <c r="W30" s="58" t="e">
+      <c r="V30" s="36"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="58" t="e">
         <f>VLOOKUP(C30,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="2:23" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="7"/>
@@ -20113,8 +20161,8 @@
       <c r="I31" s="9"/>
       <c r="J31" s="10"/>
       <c r="K31" s="9" t="e">
-        <f>IF(C31="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
-        <v>#REF!</v>
+        <f ca="1">IF(C31="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(#REF!,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(#REF!,"EQY_REC_CONS")))</f>
+        <v>#NAME?</v>
       </c>
       <c r="L31" s="11"/>
       <c r="M31" s="7"/>
@@ -20126,13 +20174,14 @@
       <c r="S31" s="36"/>
       <c r="T31" s="36"/>
       <c r="U31" s="37"/>
-      <c r="V31" s="59"/>
-      <c r="W31" s="58" t="e">
+      <c r="V31" s="36"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="58" t="e">
         <f>VLOOKUP(C31,Data!$A$2:$P$100,16,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="54">
@@ -20177,10 +20226,14 @@
         <v>9576.702850033922</v>
       </c>
       <c r="U32" s="37"/>
-      <c r="V32" s="59"/>
+      <c r="V32" s="41">
+        <f>SUM(V9:V31)</f>
+        <v>341611.23083292547</v>
+      </c>
       <c r="W32" s="59"/>
-    </row>
-    <row r="33" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X32" s="59"/>
+    </row>
+    <row r="33" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
@@ -20208,10 +20261,11 @@
       <c r="S33" s="36"/>
       <c r="T33" s="36"/>
       <c r="U33" s="37"/>
-      <c r="V33" s="59"/>
+      <c r="V33" s="36"/>
       <c r="W33" s="59"/>
-    </row>
-    <row r="34" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X33" s="59"/>
+    </row>
+    <row r="34" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="39" t="str">
         <f>IF(LEFT(C34,2) = "RU", VLOOKUP(C34,MICEX!$A:$D,4,FALSE),VLOOKUP(C34,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>RUSSIA 12 3/4 06/24/28</v>
@@ -20220,7 +20274,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="7">
-        <f>R34/$R$55</f>
+        <f>R34/$R$54</f>
         <v>0.22789061203107797</v>
       </c>
       <c r="E34" s="36">
@@ -20228,7 +20282,7 @@
         <v>449000</v>
       </c>
       <c r="F34" s="36">
-        <f t="shared" ref="F34:F38" si="15">$J$5-P34</f>
+        <f t="shared" ref="F34:F38" si="14">$J$5-P34</f>
         <v>1713692.5</v>
       </c>
       <c r="G34" s="57">
@@ -20253,11 +20307,11 @@
         <v>USD</v>
       </c>
       <c r="M34" s="7">
-        <f t="shared" ref="M34:N38" si="16">IF(O34&gt;0,Q34/O34-1,0)</f>
+        <f t="shared" ref="M34:N38" si="15">IF(O34&gt;0,Q34/O34-1,0)</f>
         <v>9.2665731747936242E-3</v>
       </c>
       <c r="N34" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4.5529706889482213E-3</v>
       </c>
       <c r="O34" s="36">
@@ -20277,24 +20331,28 @@
         <v>789887.53500000015</v>
       </c>
       <c r="S34" s="36">
-        <f t="shared" ref="S34:S38" si="17">Q34-O34</f>
+        <f t="shared" ref="S34:S38" si="16">Q34-O34</f>
         <v>429694.26271501184</v>
       </c>
       <c r="T34" s="36">
-        <f t="shared" ref="T34:T38" si="18">R34-P34</f>
+        <f t="shared" ref="T34:T38" si="17">R34-P34</f>
         <v>3580.035000000149</v>
       </c>
       <c r="U34" s="37">
         <f>VLOOKUP(C34,Data!$B:$P,14,FALSE)</f>
         <v>4.0326066999999997</v>
       </c>
-      <c r="V34" s="58" t="str">
-        <f>VLOOKUP(C34,Data!$B:$P,15,FALSE)</f>
+      <c r="V34" s="36">
+        <f>VLOOKUP(C34,Data!$B:$P,5,FALSE)/VLOOKUP(C34,Data!$B:$P,2,FALSE)*(  VLOOKUP(C34,Data!$B:$P,2,FALSE) + VLOOKUP(C34,Data!$B:$P,12,FALSE))</f>
+        <v>799110.74333333352</v>
+      </c>
+      <c r="W34" s="58" t="str">
+        <f>IF(VLOOKUP(C34,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C34,Data!$B:$P,15,FALSE))</f>
         <v>24/12/2017</v>
       </c>
-      <c r="W34" s="59"/>
-    </row>
-    <row r="35" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X34" s="59"/>
+    </row>
+    <row r="35" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="39" t="str">
         <f>IF(LEFT(C35,2) = "RU", VLOOKUP(C35,MICEX!$A:$D,4,FALSE),VLOOKUP(C35,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>GLPRLI 6.872 01/25/22</v>
@@ -20303,7 +20361,7 @@
         <v>4958</v>
       </c>
       <c r="D35" s="7">
-        <f>R35/$R$55</f>
+        <f>R35/$R$54</f>
         <v>6.0836472870082224E-2</v>
       </c>
       <c r="E35" s="36">
@@ -20311,7 +20369,7 @@
         <v>200000</v>
       </c>
       <c r="F35" s="36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2289300</v>
       </c>
       <c r="G35" s="57">
@@ -20336,11 +20394,11 @@
         <v>USD</v>
       </c>
       <c r="M35" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4.0801204210043629E-2</v>
       </c>
       <c r="N35" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>7.7930707166595781E-4</v>
       </c>
       <c r="O35" s="36">
@@ -20360,24 +20418,28 @@
         <v>210864.2</v>
       </c>
       <c r="S35" s="36">
+        <f t="shared" si="16"/>
+        <v>489766.49580000155</v>
+      </c>
+      <c r="T35" s="36">
         <f t="shared" si="17"/>
-        <v>489766.49580000155</v>
-      </c>
-      <c r="T35" s="36">
-        <f t="shared" si="18"/>
         <v>164.20000000001164</v>
       </c>
       <c r="U35" s="37">
         <f>VLOOKUP(C35,Data!$B:$P,14,FALSE)</f>
         <v>5.4715489999999996</v>
       </c>
-      <c r="V35" s="58" t="str">
-        <f>VLOOKUP(C35,Data!$B:$P,15,FALSE)</f>
+      <c r="V35" s="36">
+        <f>VLOOKUP(C35,Data!$B:$P,5,FALSE)/VLOOKUP(C35,Data!$B:$P,2,FALSE)*(  VLOOKUP(C35,Data!$B:$P,2,FALSE) + VLOOKUP(C35,Data!$B:$P,12,FALSE))</f>
+        <v>211895</v>
+      </c>
+      <c r="W35" s="58" t="str">
+        <f>IF(VLOOKUP(C35,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C35,Data!$B:$P,15,FALSE))</f>
         <v>25/01/2018</v>
       </c>
-      <c r="W35" s="59"/>
-    </row>
-    <row r="36" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X35" s="59"/>
+    </row>
+    <row r="36" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="39" t="str">
         <f>IF(LEFT(C36,2) = "RU", VLOOKUP(C36,MICEX!$A:$D,4,FALSE),VLOOKUP(C36,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>MRFGBZ 8 06/08/23</v>
@@ -20386,7 +20448,7 @@
         <v>5027</v>
       </c>
       <c r="D36" s="7">
-        <f>R36/$R$55</f>
+        <f>R36/$R$54</f>
         <v>6.0558175929537154E-2</v>
       </c>
       <c r="E36" s="36">
@@ -20394,7 +20456,7 @@
         <v>200000</v>
       </c>
       <c r="F36" s="36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2293000</v>
       </c>
       <c r="G36" s="57">
@@ -20419,11 +20481,11 @@
         <v>USD</v>
       </c>
       <c r="M36" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4.2385730503244901E-2</v>
       </c>
       <c r="N36" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>1.4007729468598962E-2</v>
       </c>
       <c r="O36" s="36">
@@ -20443,24 +20505,28 @@
         <v>209899.59999999998</v>
       </c>
       <c r="S36" s="36">
+        <f t="shared" si="16"/>
+        <v>505689.40039999969</v>
+      </c>
+      <c r="T36" s="36">
         <f t="shared" si="17"/>
-        <v>505689.40039999969</v>
-      </c>
-      <c r="T36" s="36">
-        <f t="shared" si="18"/>
         <v>2899.5999999999767</v>
       </c>
       <c r="U36" s="37">
         <f>VLOOKUP(C36,Data!$B:$P,14,FALSE)</f>
         <v>6.5013044000000004</v>
       </c>
-      <c r="V36" s="58" t="str">
-        <f>VLOOKUP(C36,Data!$B:$P,15,FALSE)</f>
+      <c r="V36" s="36">
+        <f>VLOOKUP(C36,Data!$B:$P,5,FALSE)/VLOOKUP(C36,Data!$B:$P,2,FALSE)*(  VLOOKUP(C36,Data!$B:$P,2,FALSE) + VLOOKUP(C36,Data!$B:$P,12,FALSE))</f>
+        <v>213232.93333333332</v>
+      </c>
+      <c r="W36" s="58" t="str">
+        <f>IF(VLOOKUP(C36,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C36,Data!$B:$P,15,FALSE))</f>
         <v>08/12/2017</v>
       </c>
-      <c r="W36" s="59"/>
-    </row>
-    <row r="37" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X36" s="59"/>
+    </row>
+    <row r="37" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="39" t="str">
         <f>IF(LEFT(C37,2) = "RU", VLOOKUP(C37,MICEX!$A:$D,4,FALSE),VLOOKUP(C37,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>JBSSBZ 7 3/4 10/28/20</v>
@@ -20469,7 +20535,7 @@
         <v>4847</v>
       </c>
       <c r="D37" s="7">
-        <f>R37/$R$55</f>
+        <f>R37/$R$54</f>
         <v>5.8781760915724145E-2</v>
       </c>
       <c r="E37" s="36">
@@ -20477,7 +20543,7 @@
         <v>200000</v>
       </c>
       <c r="F37" s="36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2291500</v>
       </c>
       <c r="G37" s="57">
@@ -20502,11 +20568,11 @@
         <v>USD</v>
       </c>
       <c r="M37" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>4.5291651417569412E-3</v>
       </c>
       <c r="N37" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>-2.2818225419664273E-2</v>
       </c>
       <c r="O37" s="36">
@@ -20526,24 +20592,28 @@
         <v>203742.4</v>
       </c>
       <c r="S37" s="36">
+        <f t="shared" si="16"/>
+        <v>54427.457599999383</v>
+      </c>
+      <c r="T37" s="36">
         <f t="shared" si="17"/>
-        <v>54427.457599999383</v>
-      </c>
-      <c r="T37" s="36">
-        <f t="shared" si="18"/>
         <v>-4757.6000000000058</v>
       </c>
       <c r="U37" s="37">
         <f>VLOOKUP(C37,Data!$B:$P,14,FALSE)</f>
         <v>6.8047332000000003</v>
       </c>
-      <c r="V37" s="58" t="str">
-        <f>VLOOKUP(C37,Data!$B:$P,15,FALSE)</f>
+      <c r="V37" s="36">
+        <f>VLOOKUP(C37,Data!$B:$P,5,FALSE)/VLOOKUP(C37,Data!$B:$P,2,FALSE)*(  VLOOKUP(C37,Data!$B:$P,2,FALSE) + VLOOKUP(C37,Data!$B:$P,12,FALSE))</f>
+        <v>208693.7888888889</v>
+      </c>
+      <c r="W37" s="58" t="str">
+        <f>IF(VLOOKUP(C37,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C37,Data!$B:$P,15,FALSE))</f>
         <v>28/10/2017</v>
       </c>
-      <c r="W37" s="59"/>
-    </row>
-    <row r="38" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X37" s="59"/>
+    </row>
+    <row r="38" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="39" t="str">
         <f>IF(LEFT(C38,2) = "RU", VLOOKUP(C38,MICEX!$A:$D,4,FALSE),VLOOKUP(C38,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>KAZNMH 4 5/8 05/24/23</v>
@@ -20552,7 +20622,7 @@
         <v>5023</v>
       </c>
       <c r="D38" s="7">
-        <f>R38/$R$55</f>
+        <f>R38/$R$54</f>
         <v>5.7658590700565629E-2</v>
       </c>
       <c r="E38" s="36">
@@ -20560,7 +20630,7 @@
         <v>200000</v>
       </c>
       <c r="F38" s="36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2304600</v>
       </c>
       <c r="G38" s="57">
@@ -20585,11 +20655,11 @@
         <v>USD</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.0023606061745367E-2</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>2.2770726714432143E-2</v>
       </c>
       <c r="O38" s="36">
@@ -20609,24 +20679,28 @@
         <v>199849.40000000002</v>
       </c>
       <c r="S38" s="36">
+        <f t="shared" si="16"/>
+        <v>345143.38060000166</v>
+      </c>
+      <c r="T38" s="36">
         <f t="shared" si="17"/>
-        <v>345143.38060000166</v>
-      </c>
-      <c r="T38" s="36">
-        <f t="shared" si="18"/>
         <v>4449.4000000000233</v>
       </c>
       <c r="U38" s="37">
         <f>VLOOKUP(C38,Data!$B:$P,14,FALSE)</f>
         <v>4.6387727999999999</v>
       </c>
-      <c r="V38" s="58" t="str">
-        <f>VLOOKUP(C38,Data!$B:$P,15,FALSE)</f>
+      <c r="V38" s="36">
+        <f>VLOOKUP(C38,Data!$B:$P,5,FALSE)/VLOOKUP(C38,Data!$B:$P,2,FALSE)*(  VLOOKUP(C38,Data!$B:$P,2,FALSE) + VLOOKUP(C38,Data!$B:$P,12,FALSE))</f>
+        <v>202110.51111111115</v>
+      </c>
+      <c r="W38" s="58" t="str">
+        <f>IF(VLOOKUP(C38,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C38,Data!$B:$P,15,FALSE))</f>
         <v>24/11/2017</v>
       </c>
-      <c r="W38" s="59"/>
-    </row>
-    <row r="39" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="X38" s="59"/>
+    </row>
+    <row r="39" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="39" t="str">
         <f>IF(LEFT(C39,2) = "RU", VLOOKUP(C39,MICEX!$A:$D,4,FALSE),VLOOKUP(C39,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>NMOSRM 10 04/26/19</v>
@@ -20635,7 +20709,7 @@
         <v>5625</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" ref="D39:D49" si="19">R39/$R$55</f>
+        <f>R39/$R$54</f>
         <v>5.5026748708961508E-2</v>
       </c>
       <c r="E39" s="36">
@@ -20643,7 +20717,7 @@
         <v>200000</v>
       </c>
       <c r="F39" s="36">
-        <f t="shared" ref="F39:F49" si="20">$J$5-P39</f>
+        <f t="shared" ref="F39:F48" si="18">$J$5-P39</f>
         <v>2289750</v>
       </c>
       <c r="G39" s="57">
@@ -20668,11 +20742,11 @@
         <v>USD</v>
       </c>
       <c r="M39" s="7">
-        <f t="shared" ref="M39:M49" si="21">IF(O39&gt;0,Q39/O39-1,0)</f>
+        <f t="shared" ref="M39:M48" si="19">IF(O39&gt;0,Q39/O39-1,0)</f>
         <v>-0.10337672861712444</v>
       </c>
       <c r="N39" s="7">
-        <f t="shared" ref="N39:N49" si="22">IF(P39&gt;0,R39/P39-1,0)</f>
+        <f t="shared" ref="N39:N48" si="20">IF(P39&gt;0,R39/P39-1,0)</f>
         <v>-9.2855077288941823E-2</v>
       </c>
       <c r="O39" s="36">
@@ -20692,23 +20766,27 @@
         <v>190727.21999999997</v>
       </c>
       <c r="S39" s="36">
-        <f t="shared" ref="S39:S49" si="23">Q39-O39</f>
+        <f t="shared" ref="S39:S48" si="21">Q39-O39</f>
         <v>-1302886.1922200006</v>
       </c>
       <c r="T39" s="36">
-        <f t="shared" ref="T39:T49" si="24">R39-P39</f>
+        <f t="shared" ref="T39:T48" si="22">R39-P39</f>
         <v>-19522.780000000028</v>
       </c>
       <c r="U39" s="37">
         <f>VLOOKUP(C39,Data!$B:$P,14,FALSE)</f>
         <v>13.143872500000001</v>
       </c>
-      <c r="V39" s="58" t="str">
-        <f>VLOOKUP(C39,Data!$B:$P,15,FALSE)</f>
+      <c r="V39" s="36">
+        <f>VLOOKUP(C39,Data!$B:$P,5,FALSE)/VLOOKUP(C39,Data!$B:$P,2,FALSE)*(  VLOOKUP(C39,Data!$B:$P,2,FALSE) + VLOOKUP(C39,Data!$B:$P,12,FALSE))</f>
+        <v>197171.66444444441</v>
+      </c>
+      <c r="W39" s="58" t="str">
+        <f>IF(VLOOKUP(C39,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C39,Data!$B:$P,15,FALSE))</f>
         <v>26/10/2017</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="39" t="str">
         <f>IF(LEFT(C40,2) = "RU", VLOOKUP(C40,MICEX!$A:$D,4,FALSE),VLOOKUP(C40,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>AFKSRU 6.95 05/17/19</v>
@@ -20717,7 +20795,7 @@
         <v>5775</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" si="19"/>
+        <f>R40/$R$54</f>
         <v>5.2645506678540732E-2</v>
       </c>
       <c r="E40" s="36">
@@ -20725,7 +20803,7 @@
         <v>200000</v>
       </c>
       <c r="F40" s="36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2321700</v>
       </c>
       <c r="G40" s="57">
@@ -20750,11 +20828,11 @@
         <v>USD</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>2.6295497387258671E-2</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>2.3407964105440104E-2</v>
       </c>
       <c r="O40" s="36">
@@ -20774,23 +20852,27 @@
         <v>182473.63999999998</v>
       </c>
       <c r="S40" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>277006.60636000149</v>
       </c>
       <c r="T40" s="36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>4173.6399999999849</v>
       </c>
       <c r="U40" s="37">
         <f>VLOOKUP(C40,Data!$B:$P,14,FALSE)</f>
         <v>12.715666000000001</v>
       </c>
-      <c r="V40" s="58" t="str">
-        <f>VLOOKUP(C40,Data!$B:$P,15,FALSE)</f>
+      <c r="V40" s="36">
+        <f>VLOOKUP(C40,Data!$B:$P,5,FALSE)/VLOOKUP(C40,Data!$B:$P,2,FALSE)*(  VLOOKUP(C40,Data!$B:$P,2,FALSE) + VLOOKUP(C40,Data!$B:$P,12,FALSE))</f>
+        <v>186141.69555555555</v>
+      </c>
+      <c r="W40" s="58" t="str">
+        <f>IF(VLOOKUP(C40,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C40,Data!$B:$P,15,FALSE))</f>
         <v>17/11/2017</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="39" t="str">
         <f>IF(LEFT(C41,2) = "RU", VLOOKUP(C41,MICEX!$A:$D,4,FALSE),VLOOKUP(C41,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>PETBRA 8 3/4 05/23/26</v>
@@ -20799,7 +20881,7 @@
         <v>5571</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="19"/>
+        <f>R41/$R$54</f>
         <v>3.4019132262267805E-2</v>
       </c>
       <c r="E41" s="36">
@@ -20807,7 +20889,7 @@
         <v>100000</v>
       </c>
       <c r="F41" s="36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2384750</v>
       </c>
       <c r="G41" s="57">
@@ -20832,11 +20914,11 @@
         <v>USD</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>6.0494470368590125E-2</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>2.3107158351409973E-2</v>
       </c>
       <c r="O41" s="36">
@@ -20856,23 +20938,27 @@
         <v>117913.09999999999</v>
       </c>
       <c r="S41" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>398520.21189999953</v>
       </c>
       <c r="T41" s="36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>2663.0999999999913</v>
       </c>
       <c r="U41" s="37">
         <f>VLOOKUP(C41,Data!$B:$P,14,FALSE)</f>
         <v>6.0777428000000002</v>
       </c>
-      <c r="V41" s="58" t="str">
-        <f>VLOOKUP(C41,Data!$B:$P,15,FALSE)</f>
+      <c r="V41" s="36">
+        <f>VLOOKUP(C41,Data!$B:$P,5,FALSE)/VLOOKUP(C41,Data!$B:$P,2,FALSE)*(  VLOOKUP(C41,Data!$B:$P,2,FALSE) + VLOOKUP(C41,Data!$B:$P,12,FALSE))</f>
+        <v>120100.59999999999</v>
+      </c>
+      <c r="W41" s="58" t="str">
+        <f>IF(VLOOKUP(C41,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C41,Data!$B:$P,15,FALSE))</f>
         <v>23/11/2017</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="39" t="str">
         <f>IF(LEFT(C42,2) = "RU", VLOOKUP(C42,MICEX!$A:$D,4,FALSE),VLOOKUP(C42,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>EFGBNK 0 01/04/19</v>
@@ -20881,7 +20967,7 @@
         <v>5690</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="19"/>
+        <f>R42/$R$54</f>
         <v>2.8669258741408316E-2</v>
       </c>
       <c r="E42" s="36">
@@ -20889,7 +20975,7 @@
         <v>100000</v>
       </c>
       <c r="F42" s="36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2400000</v>
       </c>
       <c r="G42" s="57">
@@ -20914,11 +21000,11 @@
         <v>USD</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>-8.5957461497787602E-3</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-6.2999999999998613E-3</v>
       </c>
       <c r="O42" s="36">
@@ -20938,23 +21024,27 @@
         <v>99370.000000000015</v>
       </c>
       <c r="S42" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>-51046.86999999918</v>
       </c>
       <c r="T42" s="36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>-629.99999999998545</v>
       </c>
       <c r="U42" s="37">
         <f>VLOOKUP(C42,Data!$B:$P,14,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="V42" s="58" t="str">
-        <f>VLOOKUP(C42,Data!$B:$P,15,FALSE)</f>
+      <c r="V42" s="36">
+        <f>VLOOKUP(C42,Data!$B:$P,5,FALSE)/VLOOKUP(C42,Data!$B:$P,2,FALSE)*(  VLOOKUP(C42,Data!$B:$P,2,FALSE) + VLOOKUP(C42,Data!$B:$P,12,FALSE))</f>
+        <v>99370.000000000015</v>
+      </c>
+      <c r="W42" s="58" t="str">
+        <f>IF(VLOOKUP(C42,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C42,Data!$B:$P,15,FALSE))</f>
         <v>03/10/2017</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="39" t="str">
         <f>IF(LEFT(C43,2) = "RU", VLOOKUP(C43,MICEX!$A:$D,4,FALSE),VLOOKUP(C43,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>EFGBNK 0 01/10/22</v>
@@ -20963,7 +21053,7 @@
         <v>5029</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="19"/>
+        <f>R43/$R$54</f>
         <v>2.8077812827954678E-2</v>
       </c>
       <c r="E43" s="36">
@@ -20971,7 +21061,7 @@
         <v>100000</v>
       </c>
       <c r="F43" s="36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2400000</v>
       </c>
       <c r="G43" s="57">
@@ -20996,11 +21086,11 @@
         <v>USD</v>
       </c>
       <c r="M43" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>-1.1585669472204851E-2</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>-2.6800000000000157E-2</v>
       </c>
       <c r="O43" s="36">
@@ -21020,23 +21110,27 @@
         <v>97319.999999999985</v>
       </c>
       <c r="S43" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>-67587.320000001229</v>
       </c>
       <c r="T43" s="36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>-2680.0000000000146</v>
       </c>
       <c r="U43" s="37">
         <f>VLOOKUP(C43,Data!$B:$P,14,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="V43" s="58">
-        <f>VLOOKUP(C43,Data!$B:$P,15,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V43" s="36">
+        <f>VLOOKUP(C43,Data!$B:$P,5,FALSE)/VLOOKUP(C43,Data!$B:$P,2,FALSE)*(  VLOOKUP(C43,Data!$B:$P,2,FALSE) + VLOOKUP(C43,Data!$B:$P,12,FALSE))</f>
+        <v>97319.999999999985</v>
+      </c>
+      <c r="W43" s="58" t="str">
+        <f>IF(VLOOKUP(C43,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C43,Data!$B:$P,15,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="39" t="str">
         <f>IF(LEFT(C44,2) = "RU", VLOOKUP(C44,MICEX!$A:$D,4,FALSE),VLOOKUP(C44,BloombergSecs!$A:$C,3,FALSE))</f>
         <v>KNFP 0 04/15/19</v>
@@ -21045,7 +21139,7 @@
         <v>5046</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="19"/>
+        <f>R44/$R$54</f>
         <v>1.4193836392282024E-2</v>
       </c>
       <c r="E44" s="36">
@@ -21053,7 +21147,7 @@
         <v>50000</v>
       </c>
       <c r="F44" s="36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2452500</v>
       </c>
       <c r="G44" s="57">
@@ -21078,11 +21172,11 @@
         <v>USD</v>
       </c>
       <c r="M44" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>8.1557757003832165E-2</v>
       </c>
       <c r="N44" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>3.5726315789473606E-2</v>
       </c>
       <c r="O44" s="36">
@@ -21102,139 +21196,147 @@
         <v>49197</v>
       </c>
       <c r="S44" s="36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>219803.80300000031</v>
       </c>
       <c r="T44" s="36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>1697</v>
       </c>
       <c r="U44" s="37">
         <f>VLOOKUP(C44,Data!$B:$P,14,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="V44" s="58" t="str">
-        <f>VLOOKUP(C44,Data!$B:$P,15,FALSE)</f>
+      <c r="V44" s="36">
+        <f>VLOOKUP(C44,Data!$B:$P,5,FALSE)/VLOOKUP(C44,Data!$B:$P,2,FALSE)*(  VLOOKUP(C44,Data!$B:$P,2,FALSE) + VLOOKUP(C44,Data!$B:$P,12,FALSE))</f>
+        <v>49197</v>
+      </c>
+      <c r="W44" s="58" t="str">
+        <f>IF(VLOOKUP(C44,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C44,Data!$B:$P,15,FALSE))</f>
         <v>14/07/2017</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="39" t="str">
         <f>IF(LEFT(C45,2) = "RU", VLOOKUP(C45,MICEX!$A:$D,4,FALSE),VLOOKUP(C45,BloombergSecs!$A:$C,3,FALSE))</f>
-        <v>MTNSJ 4.755 11/11/24</v>
+        <v>PETBRA 4 3/4 01/14/25</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>5892</v>
+        <v>5667</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f>R45/$R$54</f>
+        <v>3.5542222752892073E-2</v>
       </c>
       <c r="E45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,4,FALSE)</f>
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="F45" s="36">
-        <f t="shared" si="20"/>
-        <v>2304000</v>
+        <f t="shared" si="18"/>
+        <v>2384675.7949531325</v>
       </c>
       <c r="G45" s="57">
         <f>VLOOKUP(C45,Data!$B:$P,3,FALSE)</f>
-        <v>98</v>
+        <v>103.3</v>
       </c>
       <c r="H45" s="56">
         <f>VLOOKUP(C45,Data!$B:$P,2,FALSE)</f>
-        <v>0</v>
+        <v>104.791</v>
       </c>
       <c r="I45" s="9">
         <f>VLOOKUP(C45,Data!$B:$P,13,FALSE)</f>
-        <v>0</v>
+        <v>6.2697714097476167</v>
       </c>
       <c r="J45" s="7">
         <f>VLOOKUP(C45,Data!$B:$P,14,FALSE)/100</f>
-        <v>0</v>
+        <v>3.9859712999999998E-2</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="11" t="str">
         <f>VLOOKUP(C45,Data!$B:$P,10,FALSE)</f>
-        <v>USD</v>
+        <v>EUR</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" si="21"/>
-        <v>-1</v>
+        <f t="shared" si="19"/>
+        <v>5.225580434093291E-2</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" si="22"/>
-        <v>-1</v>
+        <f t="shared" si="20"/>
+        <v>6.8225498669332918E-2</v>
       </c>
       <c r="O45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,8,FALSE)</f>
-        <v>11771858</v>
+        <v>6936543.3499999996</v>
       </c>
       <c r="P45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,7,FALSE)</f>
-        <v>196000</v>
+        <v>115324.20504686756</v>
       </c>
       <c r="Q45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,6,FALSE)</f>
-        <v>0</v>
+        <v>7299018.0020999992</v>
       </c>
       <c r="R45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,5,FALSE)</f>
-        <v>0</v>
+        <v>123192.25644483449</v>
       </c>
       <c r="S45" s="36">
-        <f t="shared" si="23"/>
-        <v>-11771858</v>
+        <f t="shared" si="21"/>
+        <v>362474.6520999996</v>
       </c>
       <c r="T45" s="36">
-        <f t="shared" si="24"/>
-        <v>-196000</v>
+        <f t="shared" si="22"/>
+        <v>7868.051397966934</v>
       </c>
       <c r="U45" s="37">
         <f>VLOOKUP(C45,Data!$B:$P,14,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="V45" s="58" t="str">
-        <f>VLOOKUP(C45,Data!$B:$P,15,FALSE)</f>
-        <v>18/08/2017</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>3.9859713000000001</v>
+      </c>
+      <c r="V45" s="36">
+        <f>VLOOKUP(C45,Data!$B:$P,5,FALSE)/VLOOKUP(C45,Data!$B:$P,2,FALSE)*(  VLOOKUP(C45,Data!$B:$P,2,FALSE) + VLOOKUP(C45,Data!$B:$P,12,FALSE))</f>
+        <v>126558.01416989407</v>
+      </c>
+      <c r="W45" s="58" t="str">
+        <f>IF(VLOOKUP(C45,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C45,Data!$B:$P,15,FALSE))</f>
+        <v>14/01/2018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="39" t="str">
         <f>IF(LEFT(C46,2) = "RU", VLOOKUP(C46,MICEX!$A:$D,4,FALSE),VLOOKUP(C46,BloombergSecs!$A:$C,3,FALSE))</f>
-        <v>PETBRA 4 3/4 01/14/25</v>
+        <v>EFGBNK 0 06/06/19</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>5667</v>
+        <v>5621</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="19"/>
-        <v>3.5542222752892073E-2</v>
+        <f>R46/$R$54</f>
+        <v>3.3917247428588412E-2</v>
       </c>
       <c r="E46" s="36">
         <f>VLOOKUP(C46,Data!$B:$P,4,FALSE)</f>
         <v>100000</v>
       </c>
       <c r="F46" s="36">
-        <f t="shared" si="20"/>
-        <v>2384675.7949531325</v>
+        <f t="shared" si="18"/>
+        <v>2389429.9838991207</v>
       </c>
       <c r="G46" s="57">
         <f>VLOOKUP(C46,Data!$B:$P,3,FALSE)</f>
-        <v>103.3</v>
+        <v>99</v>
       </c>
       <c r="H46" s="56">
         <f>VLOOKUP(C46,Data!$B:$P,2,FALSE)</f>
-        <v>104.791</v>
+        <v>100</v>
       </c>
       <c r="I46" s="9">
         <f>VLOOKUP(C46,Data!$B:$P,13,FALSE)</f>
-        <v>6.2697714097476167</v>
+        <v>0</v>
       </c>
       <c r="J46" s="7">
         <f>VLOOKUP(C46,Data!$B:$P,14,FALSE)/100</f>
-        <v>3.9859712999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="K46" s="9"/>
       <c r="L46" s="11" t="str">
@@ -21242,56 +21344,60 @@
         <v>EUR</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" si="21"/>
-        <v>5.225580434093291E-2</v>
+        <f t="shared" si="19"/>
+        <v>9.0814973064255122E-2</v>
       </c>
       <c r="N46" s="7">
-        <f t="shared" si="22"/>
-        <v>6.8225498669332918E-2</v>
+        <f t="shared" si="20"/>
+        <v>6.3217343756321265E-2</v>
       </c>
       <c r="O46" s="36">
         <f>VLOOKUP(C46,Data!$B:$P,8,FALSE)</f>
-        <v>6936543.3499999996</v>
+        <v>6385418.4000000004</v>
       </c>
       <c r="P46" s="36">
         <f>VLOOKUP(C46,Data!$B:$P,7,FALSE)</f>
-        <v>115324.20504686756</v>
+        <v>110570.01610087909</v>
       </c>
       <c r="Q46" s="36">
         <f>VLOOKUP(C46,Data!$B:$P,6,FALSE)</f>
-        <v>7299018.0020999992</v>
+        <v>6965310</v>
       </c>
       <c r="R46" s="36">
         <f>VLOOKUP(C46,Data!$B:$P,5,FALSE)</f>
-        <v>123192.25644483449</v>
+        <v>117559.95881787034</v>
       </c>
       <c r="S46" s="36">
-        <f t="shared" si="23"/>
-        <v>362474.6520999996</v>
+        <f t="shared" si="21"/>
+        <v>579891.59999999963</v>
       </c>
       <c r="T46" s="36">
-        <f t="shared" si="24"/>
-        <v>7868.051397966934</v>
+        <f t="shared" si="22"/>
+        <v>6989.9427169912524</v>
       </c>
       <c r="U46" s="37">
         <f>VLOOKUP(C46,Data!$B:$P,14,FALSE)</f>
-        <v>3.9859713000000001</v>
-      </c>
-      <c r="V46" s="58" t="str">
-        <f>VLOOKUP(C46,Data!$B:$P,15,FALSE)</f>
-        <v>14/01/2018</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="V46" s="36">
+        <f>VLOOKUP(C46,Data!$B:$P,5,FALSE)/VLOOKUP(C46,Data!$B:$P,2,FALSE)*(  VLOOKUP(C46,Data!$B:$P,2,FALSE) + VLOOKUP(C46,Data!$B:$P,12,FALSE))</f>
+        <v>117559.95881787034</v>
+      </c>
+      <c r="W46" s="58" t="str">
+        <f>IF(VLOOKUP(C46,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C46,Data!$B:$P,15,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="39" t="str">
         <f>IF(LEFT(C47,2) = "RU", VLOOKUP(C47,MICEX!$A:$D,4,FALSE),VLOOKUP(C47,BloombergSecs!$A:$C,3,FALSE))</f>
-        <v>EFGBNK 0 06/06/19</v>
+        <v>KNFP 0 05/27/19</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>5621</v>
+        <v>5415</v>
       </c>
       <c r="D47" s="7">
-        <f t="shared" si="19"/>
+        <f>R47/$R$54</f>
         <v>3.3917247428588412E-2</v>
       </c>
       <c r="E47" s="36">
@@ -21299,12 +21405,12 @@
         <v>100000</v>
       </c>
       <c r="F47" s="36">
-        <f t="shared" si="20"/>
-        <v>2389429.9838991207</v>
+        <f t="shared" si="18"/>
+        <v>2391139.9885039567</v>
       </c>
       <c r="G47" s="57">
         <f>VLOOKUP(C47,Data!$B:$P,3,FALSE)</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H47" s="56">
         <f>VLOOKUP(C47,Data!$B:$P,2,FALSE)</f>
@@ -21324,20 +21430,20 @@
         <v>EUR</v>
       </c>
       <c r="M47" s="7">
-        <f t="shared" si="21"/>
-        <v>9.0814973064255122E-2</v>
+        <f t="shared" si="19"/>
+        <v>0.14573833915635293</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" si="22"/>
-        <v>6.3217343756321265E-2</v>
+        <f t="shared" si="20"/>
+        <v>7.9918669879462723E-2</v>
       </c>
       <c r="O47" s="36">
         <f>VLOOKUP(C47,Data!$B:$P,8,FALSE)</f>
-        <v>6385418.4000000004</v>
+        <v>6079320</v>
       </c>
       <c r="P47" s="36">
         <f>VLOOKUP(C47,Data!$B:$P,7,FALSE)</f>
-        <v>110570.01610087909</v>
+        <v>108860.01149604352</v>
       </c>
       <c r="Q47" s="36">
         <f>VLOOKUP(C47,Data!$B:$P,6,FALSE)</f>
@@ -21348,187 +21454,136 @@
         <v>117559.95881787034</v>
       </c>
       <c r="S47" s="36">
-        <f t="shared" si="23"/>
-        <v>579891.59999999963</v>
+        <f t="shared" si="21"/>
+        <v>885990</v>
       </c>
       <c r="T47" s="36">
-        <f t="shared" si="24"/>
-        <v>6989.9427169912524</v>
+        <f t="shared" si="22"/>
+        <v>8699.9473218268249</v>
       </c>
       <c r="U47" s="37">
         <f>VLOOKUP(C47,Data!$B:$P,14,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="V47" s="58">
-        <f>VLOOKUP(C47,Data!$B:$P,15,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V47" s="36">
+        <f>VLOOKUP(C47,Data!$B:$P,5,FALSE)/VLOOKUP(C47,Data!$B:$P,2,FALSE)*(  VLOOKUP(C47,Data!$B:$P,2,FALSE) + VLOOKUP(C47,Data!$B:$P,12,FALSE))</f>
+        <v>117559.95881787034</v>
+      </c>
+      <c r="W47" s="58" t="str">
+        <f>IF(VLOOKUP(C47,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C47,Data!$B:$P,15,FALSE))</f>
+        <v>28/08/2017</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="39" t="str">
         <f>IF(LEFT(C48,2) = "RU", VLOOKUP(C48,MICEX!$A:$D,4,FALSE),VLOOKUP(C48,BloombergSecs!$A:$C,3,FALSE))</f>
-        <v>KNFP 0 05/27/19</v>
+        <v>RURAIL 2.73 02/26/21</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>5415</v>
+        <v>5025</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="19"/>
-        <v>3.3917247428588412E-2</v>
+        <f>R48/$R$54</f>
+        <v>6.2005008889224764E-2</v>
       </c>
       <c r="E48" s="36">
         <f>VLOOKUP(C48,Data!$B:$P,4,FALSE)</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="F48" s="36">
-        <f t="shared" si="20"/>
-        <v>2391139.9885039567</v>
+        <f t="shared" si="18"/>
+        <v>2297468.4495017841</v>
       </c>
       <c r="G48" s="57">
         <f>VLOOKUP(C48,Data!$B:$P,3,FALSE)</f>
-        <v>100</v>
+        <v>102.4</v>
       </c>
       <c r="H48" s="56">
         <f>VLOOKUP(C48,Data!$B:$P,2,FALSE)</f>
-        <v>100</v>
+        <v>103.75</v>
       </c>
       <c r="I48" s="9">
         <f>VLOOKUP(C48,Data!$B:$P,13,FALSE)</f>
-        <v>0</v>
+        <v>3.3585050738268984</v>
       </c>
       <c r="J48" s="7">
         <f>VLOOKUP(C48,Data!$B:$P,14,FALSE)/100</f>
-        <v>0</v>
+        <v>1.5132959000000001E-2</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="11" t="str">
         <f>VLOOKUP(C48,Data!$B:$P,10,FALSE)</f>
-        <v>EUR</v>
+        <v>CHF</v>
       </c>
       <c r="M48" s="7">
-        <f t="shared" si="21"/>
-        <v>0.14573833915635293</v>
+        <f t="shared" si="19"/>
+        <v>-3.4265814672266526E-2</v>
       </c>
       <c r="N48" s="7">
-        <f t="shared" si="22"/>
-        <v>7.9918669879462723E-2</v>
+        <f t="shared" si="20"/>
+        <v>6.1140553485488303E-2</v>
       </c>
       <c r="O48" s="36">
         <f>VLOOKUP(C48,Data!$B:$P,8,FALSE)</f>
-        <v>6079320</v>
+        <v>13185269.760000002</v>
       </c>
       <c r="P48" s="36">
         <f>VLOOKUP(C48,Data!$B:$P,7,FALSE)</f>
-        <v>108860.01149604352</v>
+        <v>202531.55049821592</v>
       </c>
       <c r="Q48" s="36">
         <f>VLOOKUP(C48,Data!$B:$P,6,FALSE)</f>
-        <v>6965310</v>
+        <v>12733465.750000002</v>
       </c>
       <c r="R48" s="36">
         <f>VLOOKUP(C48,Data!$B:$P,5,FALSE)</f>
-        <v>117559.95881787034</v>
+        <v>214914.44159395096</v>
       </c>
       <c r="S48" s="36">
-        <f t="shared" si="23"/>
-        <v>885990</v>
+        <f t="shared" si="21"/>
+        <v>-451804.00999999978</v>
       </c>
       <c r="T48" s="36">
-        <f t="shared" si="24"/>
-        <v>8699.9473218268249</v>
+        <f t="shared" si="22"/>
+        <v>12382.891095735045</v>
       </c>
       <c r="U48" s="37">
         <f>VLOOKUP(C48,Data!$B:$P,14,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="V48" s="58" t="str">
-        <f>VLOOKUP(C48,Data!$B:$P,15,FALSE)</f>
-        <v>28/08/2017</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="39" t="str">
-        <f>IF(LEFT(C49,2) = "RU", VLOOKUP(C49,MICEX!$A:$D,4,FALSE),VLOOKUP(C49,BloombergSecs!$A:$C,3,FALSE))</f>
-        <v>RURAIL 2.73 02/26/21</v>
-      </c>
-      <c r="C49" s="39" t="s">
-        <v>5025</v>
-      </c>
-      <c r="D49" s="7">
-        <f t="shared" si="19"/>
-        <v>6.2005008889224764E-2</v>
-      </c>
-      <c r="E49" s="36">
-        <f>VLOOKUP(C49,Data!$B:$P,4,FALSE)</f>
-        <v>200000</v>
-      </c>
-      <c r="F49" s="36">
-        <f t="shared" si="20"/>
-        <v>2297468.4495017841</v>
-      </c>
-      <c r="G49" s="57">
-        <f>VLOOKUP(C49,Data!$B:$P,3,FALSE)</f>
-        <v>102.4</v>
-      </c>
-      <c r="H49" s="56">
-        <f>VLOOKUP(C49,Data!$B:$P,2,FALSE)</f>
-        <v>103.75</v>
-      </c>
-      <c r="I49" s="9">
-        <f>VLOOKUP(C49,Data!$B:$P,13,FALSE)</f>
-        <v>3.3585050738268984</v>
-      </c>
-      <c r="J49" s="7">
-        <f>VLOOKUP(C49,Data!$B:$P,14,FALSE)/100</f>
-        <v>1.5132959000000001E-2</v>
-      </c>
+        <v>1.5132959000000001</v>
+      </c>
+      <c r="V48" s="36">
+        <f>VLOOKUP(C48,Data!$B:$P,5,FALSE)/VLOOKUP(C48,Data!$B:$P,2,FALSE)*(  VLOOKUP(C48,Data!$B:$P,2,FALSE) + VLOOKUP(C48,Data!$B:$P,12,FALSE))</f>
+        <v>217679.15620966881</v>
+      </c>
+      <c r="W48" s="58" t="str">
+        <f>IF(VLOOKUP(C48,Data!$B:$P,15,FALSE)=0,"",VLOOKUP(C48,Data!$B:$P,15,FALSE))</f>
+        <v>26/02/2018</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="7"/>
       <c r="K49" s="9"/>
-      <c r="L49" s="11" t="str">
-        <f>VLOOKUP(C49,Data!$B:$P,10,FALSE)</f>
-        <v>CHF</v>
-      </c>
-      <c r="M49" s="7">
-        <f t="shared" si="21"/>
-        <v>-3.4265814672266526E-2</v>
-      </c>
-      <c r="N49" s="7">
-        <f t="shared" si="22"/>
-        <v>6.1140553485488303E-2</v>
-      </c>
-      <c r="O49" s="36">
-        <f>VLOOKUP(C49,Data!$B:$P,8,FALSE)</f>
-        <v>13185269.760000002</v>
-      </c>
-      <c r="P49" s="36">
-        <f>VLOOKUP(C49,Data!$B:$P,7,FALSE)</f>
-        <v>202531.55049821592</v>
-      </c>
-      <c r="Q49" s="36">
-        <f>VLOOKUP(C49,Data!$B:$P,6,FALSE)</f>
-        <v>12733465.750000002</v>
-      </c>
-      <c r="R49" s="36">
-        <f>VLOOKUP(C49,Data!$B:$P,5,FALSE)</f>
-        <v>214914.44159395096</v>
-      </c>
-      <c r="S49" s="36">
-        <f t="shared" si="23"/>
-        <v>-451804.00999999978</v>
-      </c>
-      <c r="T49" s="36">
-        <f t="shared" si="24"/>
-        <v>12382.891095735045</v>
-      </c>
-      <c r="U49" s="37">
-        <f>VLOOKUP(C49,Data!$B:$P,14,FALSE)</f>
-        <v>1.5132959000000001</v>
-      </c>
-      <c r="V49" s="58" t="str">
-        <f>VLOOKUP(C49,Data!$B:$P,15,FALSE)</f>
-        <v>26/02/2018</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="L49" s="11"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="36"/>
+      <c r="P49" s="36"/>
+      <c r="Q49" s="36"/>
+      <c r="R49" s="36"/>
+      <c r="S49" s="36"/>
+      <c r="T49" s="36"/>
+      <c r="U49" s="37"/>
+      <c r="V49" s="36"/>
+    </row>
+    <row r="50" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
       <c r="D50" s="7"/>
@@ -21549,8 +21604,9 @@
       <c r="S50" s="36"/>
       <c r="T50" s="36"/>
       <c r="U50" s="37"/>
-    </row>
-    <row r="51" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V50" s="36"/>
+    </row>
+    <row r="51" spans="2:24" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="7"/>
@@ -21571,182 +21627,171 @@
       <c r="S51" s="36"/>
       <c r="T51" s="36"/>
       <c r="U51" s="37"/>
-    </row>
-    <row r="52" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="36"/>
+      <c r="V51" s="36"/>
+    </row>
+    <row r="52" spans="2:24" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="54">
+        <f>SUM(D34:D51)</f>
+        <v>0.84373963455769574</v>
+      </c>
+      <c r="E52" s="54"/>
       <c r="F52" s="36"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="56"/>
+      <c r="G52"/>
+      <c r="H52" s="8"/>
       <c r="I52" s="9"/>
-      <c r="J52" s="7"/>
+      <c r="J52" s="10">
+        <f>SUMPRODUCT(J34:J51,D34:D51)</f>
+        <v>4.1479783793291633E-2</v>
+      </c>
       <c r="K52" s="9"/>
       <c r="L52" s="11"/>
-      <c r="M52" s="7"/>
-      <c r="N52" s="7"/>
-      <c r="O52" s="36"/>
-      <c r="P52" s="36"/>
-      <c r="Q52" s="36"/>
-      <c r="R52" s="36"/>
-      <c r="S52" s="36"/>
-      <c r="T52" s="36"/>
-      <c r="U52" s="37"/>
-    </row>
-    <row r="53" spans="2:23" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="54">
-        <f>SUM(D34:D52)</f>
-        <v>0.84373963455769574</v>
-      </c>
-      <c r="E53" s="54"/>
-      <c r="F53" s="36"/>
-      <c r="G53"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="7">
+      <c r="M52" s="7">
         <f>SUMPRODUCT($D$34:$D$38,M34:M38)</f>
         <v>9.1581200257227317E-3</v>
       </c>
-      <c r="N53" s="7">
+      <c r="N52" s="7">
         <f>SUMPRODUCT($D$34:$D$38,N34:N38)</f>
         <v>1.9049046563616901E-3</v>
       </c>
-      <c r="O53" s="36"/>
-      <c r="P53" s="41">
-        <f>SUM(P34:P52)</f>
-        <v>3092493.283142006</v>
-      </c>
-      <c r="Q53" s="41">
-        <f>SUM(Q34:Q52)</f>
+      <c r="O52" s="36"/>
+      <c r="P52" s="41">
+        <f>SUM(P34:P51)</f>
+        <v>2896493.283142006</v>
+      </c>
+      <c r="Q52" s="41">
+        <f>SUM(Q34:Q51)</f>
         <v>173271965.13675499</v>
       </c>
-      <c r="R53" s="41">
-        <f>SUM(R34:R52)</f>
+      <c r="R52" s="41">
+        <f>SUM(R34:R51)</f>
         <v>2924470.7106745262</v>
       </c>
-      <c r="S53" s="41">
-        <f>SUM(S34:S52)</f>
-        <v>-9096774.5217449851</v>
-      </c>
-      <c r="T53" s="41">
-        <f>SUM(T34:T52)</f>
-        <v>-168022.57246747988</v>
-      </c>
-      <c r="U53" s="37"/>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B54" s="13" t="s">
+      <c r="S52" s="41">
+        <f>SUM(S34:S51)</f>
+        <v>2675083.4782550139</v>
+      </c>
+      <c r="T52" s="41">
+        <f>SUM(T34:T51)</f>
+        <v>27977.42753252016</v>
+      </c>
+      <c r="U52" s="37"/>
+      <c r="V52" s="41">
+        <f>SUM(V34:V51)</f>
+        <v>2963701.0246819705</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B53" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="14">
-        <f>R54/R55</f>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14">
+        <f>R53/R54</f>
         <v>5.7702040336939341E-2</v>
       </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15">
-        <f>R54*Data!G2/Data!F2</f>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15">
+        <f>R53*Data!G2/Data!F2</f>
         <v>11849800</v>
       </c>
-      <c r="R54" s="20">
+      <c r="R53" s="20">
         <v>200000</v>
       </c>
-      <c r="S54" s="21"/>
-      <c r="T54" s="22"/>
-      <c r="U54" s="18"/>
-      <c r="V54" s="18"/>
-      <c r="W54" s="18"/>
-    </row>
-    <row r="55" spans="2:23" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="25">
-        <f>D32+D53+D54</f>
+      <c r="S53" s="21"/>
+      <c r="T53" s="22"/>
+      <c r="U53" s="18"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="18"/>
+      <c r="X53" s="18"/>
+    </row>
+    <row r="54" spans="2:24" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="25">
+        <f>D32+D52+D53</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="E55" s="25"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="28">
-        <f>M32+M53</f>
+      <c r="E54" s="25"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="28">
+        <f>M32+M52</f>
         <v>1.3594896707922306E-2</v>
       </c>
-      <c r="N55" s="28">
-        <f>N32+N53</f>
+      <c r="N54" s="28">
+        <f>N32+N52</f>
         <v>4.832220051527559E-3</v>
       </c>
-      <c r="O55" s="29">
-        <f>SUM(O9:O54)</f>
-        <v>201797510.91709772</v>
-      </c>
-      <c r="P55" s="29">
-        <f>P32+P53+P54</f>
-        <v>3424527.8111248976</v>
-      </c>
-      <c r="Q55" s="29">
-        <f>Q32+Q53+Q54</f>
+      <c r="O54" s="29">
+        <f>SUM(O9:O53)</f>
+        <v>190025652.91709772</v>
+      </c>
+      <c r="P54" s="29">
+        <f>P32+P52+P53</f>
+        <v>3228527.8111248976</v>
+      </c>
+      <c r="Q54" s="29">
+        <f>Q32+Q52+Q53</f>
         <v>205361888.95237499</v>
       </c>
-      <c r="R55" s="29">
-        <f>R32+R53+R54</f>
+      <c r="R54" s="29">
+        <f>R32+R52+R53</f>
         <v>3466081.9415074517</v>
       </c>
-      <c r="S55" s="29">
-        <f>S32+S53+S54</f>
-        <v>-8285421.9647227004</v>
-      </c>
-      <c r="T55" s="29">
-        <f>T32+T53+T54</f>
-        <v>-158445.86961744598</v>
-      </c>
-      <c r="U55" s="28">
-        <f>SUMPRODUCT($D$9:$D$52,U9:U52)/100</f>
+      <c r="S54" s="29">
+        <f>S32+S52+S53</f>
+        <v>3486436.0352772991</v>
+      </c>
+      <c r="T54" s="29">
+        <f>T32+T52+T53</f>
+        <v>37554.130382554082</v>
+      </c>
+      <c r="U54" s="28">
+        <f>SUMPRODUCT($D$9:$D$51,U9:U51)/100</f>
         <v>4.8835612379798075E-2</v>
       </c>
-      <c r="V55" s="28"/>
-      <c r="W55" s="28"/>
-    </row>
-    <row r="56" spans="2:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="P56" s="32"/>
-      <c r="Q56" s="33"/>
-      <c r="R56" s="34"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="35"/>
-      <c r="U56" s="35"/>
-      <c r="V56" s="35"/>
-      <c r="W56" s="35"/>
+      <c r="V54" s="29"/>
+      <c r="W54" s="28"/>
+      <c r="X54" s="28"/>
+    </row>
+    <row r="55" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="P55" s="32"/>
+      <c r="Q55" s="33"/>
+      <c r="R55" s="34"/>
+      <c r="S55" s="35"/>
+      <c r="T55" s="35"/>
+      <c r="U55" s="35"/>
+      <c r="V55" s="34"/>
+      <c r="W55" s="35"/>
+      <c r="X55" s="35"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J31:J32 J53">
+  <conditionalFormatting sqref="J31:J32 J52">
     <cfRule type="dataBar" priority="236">
       <dataBar>
         <cfvo type="min"/>
@@ -21760,7 +21805,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U31:U33 U53">
+  <conditionalFormatting sqref="U31:U33 U52">
     <cfRule type="dataBar" priority="237">
       <dataBar>
         <cfvo type="min"/>
@@ -21774,7 +21819,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:N53 M31:N33">
+  <conditionalFormatting sqref="M52:N52 M31:N33">
     <cfRule type="dataBar" priority="238">
       <dataBar>
         <cfvo type="min"/>
@@ -21788,7 +21833,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:N53 M31:N33">
+  <conditionalFormatting sqref="M52:N52 M31:N33">
     <cfRule type="dataBar" priority="239">
       <dataBar>
         <cfvo type="min"/>
@@ -21802,7 +21847,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J53:J55 J31:J32">
+  <conditionalFormatting sqref="J52:J54 J31:J32">
     <cfRule type="dataBar" priority="240">
       <dataBar>
         <cfvo type="min"/>
@@ -21816,7 +21861,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:M55 M31:M33">
+  <conditionalFormatting sqref="M52:M54 M31:M33">
     <cfRule type="dataBar" priority="242">
       <dataBar>
         <cfvo type="min"/>
@@ -21830,7 +21875,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N53:N55 N31:N33">
+  <conditionalFormatting sqref="N52:N54 N31:N33">
     <cfRule type="dataBar" priority="244">
       <dataBar>
         <cfvo type="min"/>
@@ -21844,7 +21889,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U53:U54 U31:U33">
+  <conditionalFormatting sqref="U52:U53 U31:U33">
     <cfRule type="dataBar" priority="246">
       <dataBar>
         <cfvo type="min"/>
@@ -21858,7 +21903,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:N55 M7:N7 M31:N33">
+  <conditionalFormatting sqref="M52:N54 M7:N7 M31:N33">
     <cfRule type="dataBar" priority="248">
       <dataBar>
         <cfvo type="min"/>
@@ -21872,7 +21917,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N55">
+  <conditionalFormatting sqref="N54">
     <cfRule type="dataBar" priority="205">
       <dataBar>
         <cfvo type="min"/>
@@ -21886,7 +21931,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U55">
+  <conditionalFormatting sqref="U54">
     <cfRule type="dataBar" priority="203">
       <dataBar>
         <cfvo type="min"/>
@@ -21900,7 +21945,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U55">
+  <conditionalFormatting sqref="U54">
     <cfRule type="dataBar" priority="204">
       <dataBar>
         <cfvo type="min"/>
@@ -21914,7 +21959,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U55">
+  <conditionalFormatting sqref="U54">
     <cfRule type="dataBar" priority="202">
       <dataBar>
         <cfvo type="min"/>
@@ -22684,7 +22729,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U51:U52">
+  <conditionalFormatting sqref="U50:U51">
     <cfRule type="dataBar" priority="68">
       <dataBar>
         <cfvo type="min"/>
@@ -22698,7 +22743,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M51:N52">
+  <conditionalFormatting sqref="M50:N51">
     <cfRule type="dataBar" priority="69">
       <dataBar>
         <cfvo type="min"/>
@@ -22712,7 +22757,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M51:N52">
+  <conditionalFormatting sqref="M50:N51">
     <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="min"/>
@@ -22726,7 +22771,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M51:M52">
+  <conditionalFormatting sqref="M50:M51">
     <cfRule type="dataBar" priority="71">
       <dataBar>
         <cfvo type="min"/>
@@ -22740,7 +22785,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N51:N52">
+  <conditionalFormatting sqref="N50:N51">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="min"/>
@@ -22754,7 +22799,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U51:U52">
+  <conditionalFormatting sqref="U50:U51">
     <cfRule type="dataBar" priority="73">
       <dataBar>
         <cfvo type="min"/>
@@ -22768,7 +22813,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M51:N52">
+  <conditionalFormatting sqref="M50:N51">
     <cfRule type="dataBar" priority="74">
       <dataBar>
         <cfvo type="min"/>
@@ -22908,7 +22953,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U50">
+  <conditionalFormatting sqref="U49">
     <cfRule type="dataBar" priority="50">
       <dataBar>
         <cfvo type="min"/>
@@ -22922,7 +22967,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M50:N50">
+  <conditionalFormatting sqref="M49:N49">
     <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="min"/>
@@ -22936,7 +22981,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M50:N50">
+  <conditionalFormatting sqref="M49:N49">
     <cfRule type="dataBar" priority="52">
       <dataBar>
         <cfvo type="min"/>
@@ -22950,7 +22995,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M50">
+  <conditionalFormatting sqref="M49">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="min"/>
@@ -22964,7 +23009,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N50">
+  <conditionalFormatting sqref="N49">
     <cfRule type="dataBar" priority="54">
       <dataBar>
         <cfvo type="min"/>
@@ -22978,7 +23023,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U50">
+  <conditionalFormatting sqref="U49">
     <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="min"/>
@@ -22992,7 +23037,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M50:N50">
+  <conditionalFormatting sqref="M49:N49">
     <cfRule type="dataBar" priority="56">
       <dataBar>
         <cfvo type="min"/>
@@ -23006,7 +23051,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V54:W54">
+  <conditionalFormatting sqref="W53:X53">
     <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
@@ -23020,7 +23065,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V55:W55">
+  <conditionalFormatting sqref="W54:X54">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
@@ -23034,7 +23079,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V55:W55">
+  <conditionalFormatting sqref="W54:X54">
     <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
@@ -23048,7 +23093,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V55:W55">
+  <conditionalFormatting sqref="W54:X54">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
@@ -23058,146 +23103,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{9C570BE1-6AD3-40F9-8AC6-4DB1FE7FFE10}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U34:U49">
-    <cfRule type="dataBar" priority="21">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF008AEF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{37A03172-CD55-44EE-8BDF-F29243F56F04}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U34:U49">
-    <cfRule type="dataBar" priority="22">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{53DBEDB3-F0E6-46BA-93A9-F151D989D845}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:M49">
-    <cfRule type="dataBar" priority="17">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF008AEF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:M49">
-    <cfRule type="dataBar" priority="18">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2EC7118B-9095-490E-8037-AC03406BFEA6}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:M49">
-    <cfRule type="dataBar" priority="19">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5897E286-3993-40D0-AF00-964107CCC553}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M34:M49">
-    <cfRule type="dataBar" priority="20">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5BDD0AA4-6DE9-4ADD-BEB7-675899B052FD}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N49">
-    <cfRule type="dataBar" priority="13">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF008AEF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N49">
-    <cfRule type="dataBar" priority="14">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N49">
-    <cfRule type="dataBar" priority="15">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{97590315-91AF-4DC4-A5C5-489B8F434FA1}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N49">
-    <cfRule type="dataBar" priority="16">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B4C6371D-DF78-4395-95BB-08F7695351B7}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -23356,6 +23261,90 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="U34:U48">
+    <cfRule type="dataBar" priority="261">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{37A03172-CD55-44EE-8BDF-F29243F56F04}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U34:U48">
+    <cfRule type="dataBar" priority="263">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{53DBEDB3-F0E6-46BA-93A9-F151D989D845}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34:M48">
+    <cfRule type="dataBar" priority="265">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34:M48">
+    <cfRule type="dataBar" priority="267">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2EC7118B-9095-490E-8037-AC03406BFEA6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N34:N48">
+    <cfRule type="dataBar" priority="273">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N34:N48">
+    <cfRule type="dataBar" priority="275">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="10" orientation="landscape" r:id="rId1"/>
   <extLst>
@@ -23372,7 +23361,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J31:J32 J53</xm:sqref>
+          <xm:sqref>J31:J32 J52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{740018B9-C2F2-4044-831A-C9CA861CFDD4}">
@@ -23385,7 +23374,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U31:U33 U53</xm:sqref>
+          <xm:sqref>U31:U33 U52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D231AAC0-08BC-480C-8677-749E49F0D90A}">
@@ -23398,7 +23387,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M53:N53 M31:N33</xm:sqref>
+          <xm:sqref>M52:N52 M31:N33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{108BB3FB-8971-428C-8622-17429EBD3654}">
@@ -23411,7 +23400,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M53:N53 M31:N33</xm:sqref>
+          <xm:sqref>M52:N52 M31:N33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1B2E28D6-619A-407F-9631-79595E46C97F}">
@@ -23424,7 +23413,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J53:J55 J31:J32</xm:sqref>
+          <xm:sqref>J52:J54 J31:J32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{59B060A3-5169-484C-9E32-A34CEC5C7FF1}">
@@ -23437,7 +23426,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M53:M55 M31:M33</xm:sqref>
+          <xm:sqref>M52:M54 M31:M33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{725AB01A-6125-4180-85DD-3D988D931CE5}">
@@ -23450,7 +23439,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N53:N55 N31:N33</xm:sqref>
+          <xm:sqref>N52:N54 N31:N33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3AD491BA-61AA-425D-862C-BBC5E0035618}">
@@ -23463,7 +23452,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U53:U54 U31:U33</xm:sqref>
+          <xm:sqref>U52:U53 U31:U33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{00BC91CD-8F90-4273-B83B-1D9309E02ABA}">
@@ -23476,7 +23465,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M53:N55 M7:N7 M31:N33</xm:sqref>
+          <xm:sqref>M52:N54 M7:N7 M31:N33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{544FB895-45B3-41E1-A00A-34C34A6D5295}">
@@ -23489,7 +23478,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N55</xm:sqref>
+          <xm:sqref>N54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A7F7C0E5-BDA7-482B-96E2-D396F5636138}">
@@ -23502,7 +23491,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U55</xm:sqref>
+          <xm:sqref>U54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4077AED7-898C-4414-A896-234F03865C90}">
@@ -23515,7 +23504,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U55</xm:sqref>
+          <xm:sqref>U54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C80AC1E3-5948-4006-A1B4-8F9FFCC3B5C7}">
@@ -23528,7 +23517,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U55</xm:sqref>
+          <xm:sqref>U54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4647C4DF-1961-449C-822B-68C3E57CB9E7}">
@@ -24243,7 +24232,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U51:U52</xm:sqref>
+          <xm:sqref>U50:U51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C58909CC-3EE9-4F1F-B8C6-039CA96C6E0D}">
@@ -24256,7 +24245,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M51:N52</xm:sqref>
+          <xm:sqref>M50:N51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B5FA8225-FBE3-44D1-B12F-24A8664E3FD2}">
@@ -24269,7 +24258,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M51:N52</xm:sqref>
+          <xm:sqref>M50:N51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{12A5E219-C455-42E5-945D-5127C08E6A7E}">
@@ -24282,7 +24271,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M51:M52</xm:sqref>
+          <xm:sqref>M50:M51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1FBDF6B9-7BFD-4C6C-A992-E6F70E390C0F}">
@@ -24295,7 +24284,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N51:N52</xm:sqref>
+          <xm:sqref>N50:N51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BD2FBC30-AC3F-4CD7-8EBF-C27CEDC608BF}">
@@ -24308,7 +24297,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U51:U52</xm:sqref>
+          <xm:sqref>U50:U51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0856F52B-0288-4484-B891-E68D65A39C37}">
@@ -24321,7 +24310,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M51:N52</xm:sqref>
+          <xm:sqref>M50:N51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F9A454FD-AAE0-4C15-8AAF-65ED42FF2912}">
@@ -24451,7 +24440,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U50</xm:sqref>
+          <xm:sqref>U49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7BEF1E64-46AF-48A1-94AC-0E7884EA4128}">
@@ -24464,7 +24453,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M50:N50</xm:sqref>
+          <xm:sqref>M49:N49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{65FD7E3B-5F05-4743-A6F0-EA7360E17D43}">
@@ -24477,7 +24466,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M50:N50</xm:sqref>
+          <xm:sqref>M49:N49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{59E64FBA-FF6B-4442-AC9C-06B88B930A41}">
@@ -24490,7 +24479,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M50</xm:sqref>
+          <xm:sqref>M49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6063CF00-C4AA-4074-8808-D50CF05CD727}">
@@ -24503,7 +24492,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>N50</xm:sqref>
+          <xm:sqref>N49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5C38A9D6-BBA4-4667-9F40-5DDAF44AB407}">
@@ -24516,7 +24505,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>U50</xm:sqref>
+          <xm:sqref>U49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A95B5EDD-7331-46D3-9678-E875B3EE9FA6}">
@@ -24529,7 +24518,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>M50:N50</xm:sqref>
+          <xm:sqref>M49:N49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{424BE77F-4C99-446B-B1BC-6065628CF1D7}">
@@ -24542,7 +24531,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V54:W54</xm:sqref>
+          <xm:sqref>W53:X53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BEF95891-9D7A-4C3C-B28D-86E1C70D2F8F}">
@@ -24555,7 +24544,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V55:W55</xm:sqref>
+          <xm:sqref>W54:X54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{64AAF945-5ED7-4CEB-8FF6-21897840F850}">
@@ -24568,7 +24557,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V55:W55</xm:sqref>
+          <xm:sqref>W54:X54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9C570BE1-6AD3-40F9-8AC6-4DB1FE7FFE10}">
@@ -24581,137 +24570,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V55:W55</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{37A03172-CD55-44EE-8BDF-F29243F56F04}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>U34:U49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{53DBEDB3-F0E6-46BA-93A9-F151D989D845}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>U34:U49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2EC7118B-9095-490E-8037-AC03406BFEA6}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5897E286-3993-40D0-AF00-964107CCC553}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5BDD0AA4-6DE9-4ADD-BEB7-675899B052FD}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{97590315-91AF-4DC4-A5C5-489B8F434FA1}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B4C6371D-DF78-4395-95BB-08F7695351B7}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N49</xm:sqref>
+          <xm:sqref>W54:X54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8EFD676A-87DE-4793-A389-333D66B9DA7A}">
@@ -24873,7 +24732,7 @@
               <x14:cfIcon iconSet="3Arrows" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K53 K32:K33</xm:sqref>
+          <xm:sqref>K52 K32:K33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="191" id="{114ECFA3-0821-47BE-B7AB-089367875297}">
@@ -24930,7 +24789,7 @@
               <x14:cfIcon iconSet="3Arrows" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K51:K52 K34:K49</xm:sqref>
+          <xm:sqref>K50:K51 K34:K48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="57" id="{A6E7F667-E3CA-4B6B-822E-484CF02F32A1}">
@@ -24949,7 +24808,7 @@
               <x14:cfIcon iconSet="3Arrows" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>K50</xm:sqref>
+          <xm:sqref>K49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A70E0C30-2B1F-4119-859A-02C77EEA2754}">
@@ -24970,6 +24829,84 @@
           </x14:cfRule>
           <xm:sqref>K19:K23</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{37A03172-CD55-44EE-8BDF-F29243F56F04}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U34:U48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{53DBEDB3-F0E6-46BA-93A9-F151D989D845}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U34:U48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M34:M48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2EC7118B-9095-490E-8037-AC03406BFEA6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M34:M48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N34:N48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N34:N48</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -24981,12 +24918,13 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B7" sqref="B7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -47951,10 +47889,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C464"/>
+  <dimension ref="A1:C465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C464" sqref="C464"/>
+    <sheetView topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="B458" sqref="B458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53068,6 +53006,17 @@
         <v>5919</v>
       </c>
     </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>54</v>
+      </c>
+      <c r="B465" t="s">
+        <v>5920</v>
+      </c>
+      <c r="C465" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding new Bloomberg template
</commit_message>
<xml_diff>
--- a/sberweb/resources/public/templates/CLIENT_WEB.xlsx
+++ b/sberweb/resources/public/templates/CLIENT_WEB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7806" uniqueCount="5922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7809" uniqueCount="5925">
   <si>
     <t>Эмитент</t>
   </si>
@@ -17787,6 +17787,15 @@
   </si>
   <si>
     <t>Стоимость позиции по текущей цене (USD) с НКД</t>
+  </si>
+  <si>
+    <t>US55616P1049</t>
+  </si>
+  <si>
+    <t>M US Equity</t>
+  </si>
+  <si>
+    <t>Macy's Inc</t>
   </si>
 </sst>
 </file>
@@ -18965,7 +18974,7 @@
   </sheetPr>
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -20274,7 +20283,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="7">
-        <f>R34/$R$54</f>
+        <f t="shared" ref="D34:D48" si="14">R34/$R$54</f>
         <v>0.22789061203107797</v>
       </c>
       <c r="E34" s="36">
@@ -20282,7 +20291,7 @@
         <v>449000</v>
       </c>
       <c r="F34" s="36">
-        <f t="shared" ref="F34:F38" si="14">$J$5-P34</f>
+        <f t="shared" ref="F34:F38" si="15">$J$5-P34</f>
         <v>1713692.5</v>
       </c>
       <c r="G34" s="57">
@@ -20307,11 +20316,11 @@
         <v>USD</v>
       </c>
       <c r="M34" s="7">
-        <f t="shared" ref="M34:N38" si="15">IF(O34&gt;0,Q34/O34-1,0)</f>
+        <f t="shared" ref="M34:N38" si="16">IF(O34&gt;0,Q34/O34-1,0)</f>
         <v>9.2665731747936242E-3</v>
       </c>
       <c r="N34" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.5529706889482213E-3</v>
       </c>
       <c r="O34" s="36">
@@ -20331,11 +20340,11 @@
         <v>789887.53500000015</v>
       </c>
       <c r="S34" s="36">
-        <f t="shared" ref="S34:S38" si="16">Q34-O34</f>
+        <f t="shared" ref="S34:S38" si="17">Q34-O34</f>
         <v>429694.26271501184</v>
       </c>
       <c r="T34" s="36">
-        <f t="shared" ref="T34:T38" si="17">R34-P34</f>
+        <f t="shared" ref="T34:T38" si="18">R34-P34</f>
         <v>3580.035000000149</v>
       </c>
       <c r="U34" s="37">
@@ -20361,7 +20370,7 @@
         <v>4958</v>
       </c>
       <c r="D35" s="7">
-        <f>R35/$R$54</f>
+        <f t="shared" si="14"/>
         <v>6.0836472870082224E-2</v>
       </c>
       <c r="E35" s="36">
@@ -20369,7 +20378,7 @@
         <v>200000</v>
       </c>
       <c r="F35" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2289300</v>
       </c>
       <c r="G35" s="57">
@@ -20394,11 +20403,11 @@
         <v>USD</v>
       </c>
       <c r="M35" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.0801204210043629E-2</v>
       </c>
       <c r="N35" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.7930707166595781E-4</v>
       </c>
       <c r="O35" s="36">
@@ -20418,11 +20427,11 @@
         <v>210864.2</v>
       </c>
       <c r="S35" s="36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>489766.49580000155</v>
       </c>
       <c r="T35" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>164.20000000001164</v>
       </c>
       <c r="U35" s="37">
@@ -20448,7 +20457,7 @@
         <v>5027</v>
       </c>
       <c r="D36" s="7">
-        <f>R36/$R$54</f>
+        <f t="shared" si="14"/>
         <v>6.0558175929537154E-2</v>
       </c>
       <c r="E36" s="36">
@@ -20456,7 +20465,7 @@
         <v>200000</v>
       </c>
       <c r="F36" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2293000</v>
       </c>
       <c r="G36" s="57">
@@ -20481,11 +20490,11 @@
         <v>USD</v>
       </c>
       <c r="M36" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.2385730503244901E-2</v>
       </c>
       <c r="N36" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.4007729468598962E-2</v>
       </c>
       <c r="O36" s="36">
@@ -20505,11 +20514,11 @@
         <v>209899.59999999998</v>
       </c>
       <c r="S36" s="36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>505689.40039999969</v>
       </c>
       <c r="T36" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2899.5999999999767</v>
       </c>
       <c r="U36" s="37">
@@ -20535,7 +20544,7 @@
         <v>4847</v>
       </c>
       <c r="D37" s="7">
-        <f>R37/$R$54</f>
+        <f t="shared" si="14"/>
         <v>5.8781760915724145E-2</v>
       </c>
       <c r="E37" s="36">
@@ -20543,7 +20552,7 @@
         <v>200000</v>
       </c>
       <c r="F37" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2291500</v>
       </c>
       <c r="G37" s="57">
@@ -20568,11 +20577,11 @@
         <v>USD</v>
       </c>
       <c r="M37" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.5291651417569412E-3</v>
       </c>
       <c r="N37" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.2818225419664273E-2</v>
       </c>
       <c r="O37" s="36">
@@ -20592,11 +20601,11 @@
         <v>203742.4</v>
       </c>
       <c r="S37" s="36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>54427.457599999383</v>
       </c>
       <c r="T37" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-4757.6000000000058</v>
       </c>
       <c r="U37" s="37">
@@ -20622,7 +20631,7 @@
         <v>5023</v>
       </c>
       <c r="D38" s="7">
-        <f>R38/$R$54</f>
+        <f t="shared" si="14"/>
         <v>5.7658590700565629E-2</v>
       </c>
       <c r="E38" s="36">
@@ -20630,7 +20639,7 @@
         <v>200000</v>
       </c>
       <c r="F38" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2304600</v>
       </c>
       <c r="G38" s="57">
@@ -20655,11 +20664,11 @@
         <v>USD</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.0023606061745367E-2</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.2770726714432143E-2</v>
       </c>
       <c r="O38" s="36">
@@ -20679,11 +20688,11 @@
         <v>199849.40000000002</v>
       </c>
       <c r="S38" s="36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>345143.38060000166</v>
       </c>
       <c r="T38" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4449.4000000000233</v>
       </c>
       <c r="U38" s="37">
@@ -20709,7 +20718,7 @@
         <v>5625</v>
       </c>
       <c r="D39" s="7">
-        <f>R39/$R$54</f>
+        <f t="shared" si="14"/>
         <v>5.5026748708961508E-2</v>
       </c>
       <c r="E39" s="36">
@@ -20717,7 +20726,7 @@
         <v>200000</v>
       </c>
       <c r="F39" s="36">
-        <f t="shared" ref="F39:F48" si="18">$J$5-P39</f>
+        <f t="shared" ref="F39:F48" si="19">$J$5-P39</f>
         <v>2289750</v>
       </c>
       <c r="G39" s="57">
@@ -20742,11 +20751,11 @@
         <v>USD</v>
       </c>
       <c r="M39" s="7">
-        <f t="shared" ref="M39:M48" si="19">IF(O39&gt;0,Q39/O39-1,0)</f>
+        <f t="shared" ref="M39:M48" si="20">IF(O39&gt;0,Q39/O39-1,0)</f>
         <v>-0.10337672861712444</v>
       </c>
       <c r="N39" s="7">
-        <f t="shared" ref="N39:N48" si="20">IF(P39&gt;0,R39/P39-1,0)</f>
+        <f t="shared" ref="N39:N48" si="21">IF(P39&gt;0,R39/P39-1,0)</f>
         <v>-9.2855077288941823E-2</v>
       </c>
       <c r="O39" s="36">
@@ -20766,11 +20775,11 @@
         <v>190727.21999999997</v>
       </c>
       <c r="S39" s="36">
-        <f t="shared" ref="S39:S48" si="21">Q39-O39</f>
+        <f t="shared" ref="S39:S48" si="22">Q39-O39</f>
         <v>-1302886.1922200006</v>
       </c>
       <c r="T39" s="36">
-        <f t="shared" ref="T39:T48" si="22">R39-P39</f>
+        <f t="shared" ref="T39:T48" si="23">R39-P39</f>
         <v>-19522.780000000028</v>
       </c>
       <c r="U39" s="37">
@@ -20795,7 +20804,7 @@
         <v>5775</v>
       </c>
       <c r="D40" s="7">
-        <f>R40/$R$54</f>
+        <f t="shared" si="14"/>
         <v>5.2645506678540732E-2</v>
       </c>
       <c r="E40" s="36">
@@ -20803,7 +20812,7 @@
         <v>200000</v>
       </c>
       <c r="F40" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2321700</v>
       </c>
       <c r="G40" s="57">
@@ -20828,11 +20837,11 @@
         <v>USD</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2.6295497387258671E-2</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.3407964105440104E-2</v>
       </c>
       <c r="O40" s="36">
@@ -20852,11 +20861,11 @@
         <v>182473.63999999998</v>
       </c>
       <c r="S40" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>277006.60636000149</v>
       </c>
       <c r="T40" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>4173.6399999999849</v>
       </c>
       <c r="U40" s="37">
@@ -20881,7 +20890,7 @@
         <v>5571</v>
       </c>
       <c r="D41" s="7">
-        <f>R41/$R$54</f>
+        <f t="shared" si="14"/>
         <v>3.4019132262267805E-2</v>
       </c>
       <c r="E41" s="36">
@@ -20889,7 +20898,7 @@
         <v>100000</v>
       </c>
       <c r="F41" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2384750</v>
       </c>
       <c r="G41" s="57">
@@ -20914,11 +20923,11 @@
         <v>USD</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>6.0494470368590125E-2</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.3107158351409973E-2</v>
       </c>
       <c r="O41" s="36">
@@ -20938,11 +20947,11 @@
         <v>117913.09999999999</v>
       </c>
       <c r="S41" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>398520.21189999953</v>
       </c>
       <c r="T41" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2663.0999999999913</v>
       </c>
       <c r="U41" s="37">
@@ -20967,7 +20976,7 @@
         <v>5690</v>
       </c>
       <c r="D42" s="7">
-        <f>R42/$R$54</f>
+        <f t="shared" si="14"/>
         <v>2.8669258741408316E-2</v>
       </c>
       <c r="E42" s="36">
@@ -20975,7 +20984,7 @@
         <v>100000</v>
       </c>
       <c r="F42" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2400000</v>
       </c>
       <c r="G42" s="57">
@@ -21000,11 +21009,11 @@
         <v>USD</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-8.5957461497787602E-3</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-6.2999999999998613E-3</v>
       </c>
       <c r="O42" s="36">
@@ -21024,11 +21033,11 @@
         <v>99370.000000000015</v>
       </c>
       <c r="S42" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-51046.86999999918</v>
       </c>
       <c r="T42" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>-629.99999999998545</v>
       </c>
       <c r="U42" s="37">
@@ -21053,7 +21062,7 @@
         <v>5029</v>
       </c>
       <c r="D43" s="7">
-        <f>R43/$R$54</f>
+        <f t="shared" si="14"/>
         <v>2.8077812827954678E-2</v>
       </c>
       <c r="E43" s="36">
@@ -21061,7 +21070,7 @@
         <v>100000</v>
       </c>
       <c r="F43" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2400000</v>
       </c>
       <c r="G43" s="57">
@@ -21086,11 +21095,11 @@
         <v>USD</v>
       </c>
       <c r="M43" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-1.1585669472204851E-2</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-2.6800000000000157E-2</v>
       </c>
       <c r="O43" s="36">
@@ -21110,11 +21119,11 @@
         <v>97319.999999999985</v>
       </c>
       <c r="S43" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-67587.320000001229</v>
       </c>
       <c r="T43" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>-2680.0000000000146</v>
       </c>
       <c r="U43" s="37">
@@ -21139,7 +21148,7 @@
         <v>5046</v>
       </c>
       <c r="D44" s="7">
-        <f>R44/$R$54</f>
+        <f t="shared" si="14"/>
         <v>1.4193836392282024E-2</v>
       </c>
       <c r="E44" s="36">
@@ -21147,7 +21156,7 @@
         <v>50000</v>
       </c>
       <c r="F44" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2452500</v>
       </c>
       <c r="G44" s="57">
@@ -21172,11 +21181,11 @@
         <v>USD</v>
       </c>
       <c r="M44" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>8.1557757003832165E-2</v>
       </c>
       <c r="N44" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.5726315789473606E-2</v>
       </c>
       <c r="O44" s="36">
@@ -21196,11 +21205,11 @@
         <v>49197</v>
       </c>
       <c r="S44" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>219803.80300000031</v>
       </c>
       <c r="T44" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1697</v>
       </c>
       <c r="U44" s="37">
@@ -21225,7 +21234,7 @@
         <v>5667</v>
       </c>
       <c r="D45" s="7">
-        <f>R45/$R$54</f>
+        <f t="shared" si="14"/>
         <v>3.5542222752892073E-2</v>
       </c>
       <c r="E45" s="36">
@@ -21233,7 +21242,7 @@
         <v>100000</v>
       </c>
       <c r="F45" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2384675.7949531325</v>
       </c>
       <c r="G45" s="57">
@@ -21258,11 +21267,11 @@
         <v>EUR</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.225580434093291E-2</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.8225498669332918E-2</v>
       </c>
       <c r="O45" s="36">
@@ -21282,11 +21291,11 @@
         <v>123192.25644483449</v>
       </c>
       <c r="S45" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>362474.6520999996</v>
       </c>
       <c r="T45" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7868.051397966934</v>
       </c>
       <c r="U45" s="37">
@@ -21311,7 +21320,7 @@
         <v>5621</v>
       </c>
       <c r="D46" s="7">
-        <f>R46/$R$54</f>
+        <f t="shared" si="14"/>
         <v>3.3917247428588412E-2</v>
       </c>
       <c r="E46" s="36">
@@ -21319,7 +21328,7 @@
         <v>100000</v>
       </c>
       <c r="F46" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2389429.9838991207</v>
       </c>
       <c r="G46" s="57">
@@ -21344,11 +21353,11 @@
         <v>EUR</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0814973064255122E-2</v>
       </c>
       <c r="N46" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.3217343756321265E-2</v>
       </c>
       <c r="O46" s="36">
@@ -21368,11 +21377,11 @@
         <v>117559.95881787034</v>
       </c>
       <c r="S46" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>579891.59999999963</v>
       </c>
       <c r="T46" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6989.9427169912524</v>
       </c>
       <c r="U46" s="37">
@@ -21397,7 +21406,7 @@
         <v>5415</v>
       </c>
       <c r="D47" s="7">
-        <f>R47/$R$54</f>
+        <f t="shared" si="14"/>
         <v>3.3917247428588412E-2</v>
       </c>
       <c r="E47" s="36">
@@ -21405,7 +21414,7 @@
         <v>100000</v>
       </c>
       <c r="F47" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2391139.9885039567</v>
       </c>
       <c r="G47" s="57">
@@ -21430,11 +21439,11 @@
         <v>EUR</v>
       </c>
       <c r="M47" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.14573833915635293</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7.9918669879462723E-2</v>
       </c>
       <c r="O47" s="36">
@@ -21454,11 +21463,11 @@
         <v>117559.95881787034</v>
       </c>
       <c r="S47" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>885990</v>
       </c>
       <c r="T47" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8699.9473218268249</v>
       </c>
       <c r="U47" s="37">
@@ -21483,7 +21492,7 @@
         <v>5025</v>
       </c>
       <c r="D48" s="7">
-        <f>R48/$R$54</f>
+        <f t="shared" si="14"/>
         <v>6.2005008889224764E-2</v>
       </c>
       <c r="E48" s="36">
@@ -21491,7 +21500,7 @@
         <v>200000</v>
       </c>
       <c r="F48" s="36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2297468.4495017841</v>
       </c>
       <c r="G48" s="57">
@@ -21516,11 +21525,11 @@
         <v>CHF</v>
       </c>
       <c r="M48" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-3.4265814672266526E-2</v>
       </c>
       <c r="N48" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.1140553485488303E-2</v>
       </c>
       <c r="O48" s="36">
@@ -21540,11 +21549,11 @@
         <v>214914.44159395096</v>
       </c>
       <c r="S48" s="36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-451804.00999999978</v>
       </c>
       <c r="T48" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>12382.891095735045</v>
       </c>
       <c r="U48" s="37">
@@ -24716,6 +24725,84 @@
           <xm:sqref>J19:J23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{37A03172-CD55-44EE-8BDF-F29243F56F04}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U34:U48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{53DBEDB3-F0E6-46BA-93A9-F151D989D845}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>U34:U48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M34:M48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2EC7118B-9095-490E-8037-AC03406BFEA6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M34:M48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N34:N48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>N34:N48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="250" id="{EF154165-A510-48D6-8441-6E52AFB69160}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
@@ -24829,84 +24916,6 @@
           </x14:cfRule>
           <xm:sqref>K19:K23</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{37A03172-CD55-44EE-8BDF-F29243F56F04}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>U34:U48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{53DBEDB3-F0E6-46BA-93A9-F151D989D845}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>U34:U48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B740C84E-5F03-4F37-A03A-10F8B50DBEA1}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2EC7118B-9095-490E-8037-AC03406BFEA6}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>M34:M48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{68DC8697-ABAA-4D41-9623-BE17B35DE3BE}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF008AEF"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N48</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4FFC26DD-82EF-4613-9B31-5E9ACB2876BA}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N34:N48</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -47889,10 +47898,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C465"/>
+  <dimension ref="A1:C466"/>
   <sheetViews>
-    <sheetView topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="B458" sqref="B458"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="C452" sqref="C452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53017,6 +53026,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>5922</v>
+      </c>
+      <c r="B466" t="s">
+        <v>5923</v>
+      </c>
+      <c r="C466" t="s">
+        <v>5924</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding currency and Value date to Excel Arena parser
</commit_message>
<xml_diff>
--- a/sberweb/resources/public/templates/CLIENT_WEB.xlsx
+++ b/sberweb/resources/public/templates/CLIENT_WEB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="23580" windowHeight="14505"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -18874,11 +18874,11 @@
   </sheetPr>
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19048,7 +19048,7 @@
       </c>
       <c r="D6" s="7">
         <f>R6/$R$51</f>
-        <v>3.0510877060802067E-2</v>
+        <v>3.2379224371569162E-2</v>
       </c>
       <c r="E6" s="36">
         <f>VLOOKUP(C6,Data!$B:$P,4,FALSE)</f>
@@ -19141,7 +19141,7 @@
       </c>
       <c r="D7" s="7">
         <f>R7/$R$51</f>
-        <v>1.4098916535927758E-2</v>
+        <v>1.4962270045633056E-2</v>
       </c>
       <c r="E7" s="36">
         <f>VLOOKUP(C7,Data!$B:$P,4,FALSE)</f>
@@ -19234,7 +19234,7 @@
       </c>
       <c r="D8" s="7">
         <f>R8/$R$51</f>
-        <v>2.1862026021007133E-2</v>
+        <v>2.3200757039550823E-2</v>
       </c>
       <c r="E8" s="36">
         <f>VLOOKUP(C8,Data!$B:$P,4,FALSE)</f>
@@ -19327,7 +19327,7 @@
       </c>
       <c r="D9" s="7">
         <f>R9/$R$51</f>
-        <v>1.5114077453630201E-2</v>
+        <v>1.6039594799753757E-2</v>
       </c>
       <c r="E9" s="36">
         <f>VLOOKUP(C9,Data!$B:$P,4,FALSE)</f>
@@ -19420,7 +19420,7 @@
       </c>
       <c r="D10" s="7">
         <f>R10/$R$51</f>
-        <v>1.6972428033997643E-2</v>
+        <v>1.8011742315632844E-2</v>
       </c>
       <c r="E10" s="36">
         <f>VLOOKUP(C10,Data!$B:$P,4,FALSE)</f>
@@ -20010,7 +20010,7 @@
       <c r="C29" s="38"/>
       <c r="D29" s="43">
         <f>SUM(D6:D28)</f>
-        <v>9.8558325105364802E-2</v>
+        <v>0.10459358857213963</v>
       </c>
       <c r="E29" s="43"/>
       <c r="F29" s="36"/>
@@ -20022,11 +20022,11 @@
       <c r="L29" s="11"/>
       <c r="M29" s="7">
         <f>SUMPRODUCT($D$6:$D$20,M6:M20)</f>
-        <v>4.4367766821995745E-3</v>
+        <v>4.7084647023814437E-3</v>
       </c>
       <c r="N29" s="7">
         <f>SUMPRODUCT($D$6:$D$20,N6:N20)</f>
-        <v>2.927315395165869E-3</v>
+        <v>3.1065708729886197E-3</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="40">
@@ -20099,7 +20099,7 @@
       </c>
       <c r="D31" s="7">
         <f t="shared" ref="D31:D45" si="11">R31/$R$51</f>
-        <v>0.22789061203107797</v>
+        <v>0.24184559638924111</v>
       </c>
       <c r="E31" s="36">
         <f>VLOOKUP(C31,Data!$B:$P,4,FALSE)</f>
@@ -20186,7 +20186,7 @@
       </c>
       <c r="D32" s="7">
         <f t="shared" si="11"/>
-        <v>6.0836472870082224E-2</v>
+        <v>6.456182171065683E-2</v>
       </c>
       <c r="E32" s="36">
         <f>VLOOKUP(C32,Data!$B:$P,4,FALSE)</f>
@@ -20273,7 +20273,7 @@
       </c>
       <c r="D33" s="7">
         <f t="shared" si="11"/>
-        <v>6.0558175929537154E-2</v>
+        <v>6.4266483131504459E-2</v>
       </c>
       <c r="E33" s="36">
         <f>VLOOKUP(C33,Data!$B:$P,4,FALSE)</f>
@@ -20360,7 +20360,7 @@
       </c>
       <c r="D34" s="7">
         <f t="shared" si="11"/>
-        <v>5.8781760915724145E-2</v>
+        <v>6.2381288543533364E-2</v>
       </c>
       <c r="E34" s="36">
         <f>VLOOKUP(C34,Data!$B:$P,4,FALSE)</f>
@@ -20447,7 +20447,7 @@
       </c>
       <c r="D35" s="7">
         <f t="shared" si="11"/>
-        <v>5.7658590700565629E-2</v>
+        <v>6.1189340493937532E-2</v>
       </c>
       <c r="E35" s="36">
         <f>VLOOKUP(C35,Data!$B:$P,4,FALSE)</f>
@@ -20534,7 +20534,7 @@
       </c>
       <c r="D36" s="7">
         <f t="shared" si="11"/>
-        <v>5.5026748708961508E-2</v>
+        <v>5.8396336471573738E-2</v>
       </c>
       <c r="E36" s="36">
         <f>VLOOKUP(C36,Data!$B:$P,4,FALSE)</f>
@@ -20620,7 +20620,7 @@
       </c>
       <c r="D37" s="7">
         <f t="shared" si="11"/>
-        <v>5.2645506678540732E-2</v>
+        <v>5.5869278011983908E-2</v>
       </c>
       <c r="E37" s="36">
         <f>VLOOKUP(C37,Data!$B:$P,4,FALSE)</f>
@@ -20706,7 +20706,7 @@
       </c>
       <c r="D38" s="7">
         <f t="shared" si="11"/>
-        <v>3.4019132262267805E-2</v>
+        <v>3.6102309161777341E-2</v>
       </c>
       <c r="E38" s="36">
         <f>VLOOKUP(C38,Data!$B:$P,4,FALSE)</f>
@@ -20792,7 +20792,7 @@
       </c>
       <c r="D39" s="7">
         <f t="shared" si="11"/>
-        <v>2.8669258741408316E-2</v>
+        <v>3.0424833724207193E-2</v>
       </c>
       <c r="E39" s="36">
         <f>VLOOKUP(C39,Data!$B:$P,4,FALSE)</f>
@@ -20878,7 +20878,7 @@
       </c>
       <c r="D40" s="7">
         <f t="shared" si="11"/>
-        <v>2.8077812827954678E-2</v>
+        <v>2.9797170353626275E-2</v>
       </c>
       <c r="E40" s="36">
         <f>VLOOKUP(C40,Data!$B:$P,4,FALSE)</f>
@@ -20964,7 +20964,7 @@
       </c>
       <c r="D41" s="7">
         <f t="shared" si="11"/>
-        <v>1.4193836392282024E-2</v>
+        <v>1.5063002362179943E-2</v>
       </c>
       <c r="E41" s="36">
         <f>VLOOKUP(C41,Data!$B:$P,4,FALSE)</f>
@@ -21050,7 +21050,7 @@
       </c>
       <c r="D42" s="7">
         <f t="shared" si="11"/>
-        <v>3.5542222752892073E-2</v>
+        <v>3.7718666785186483E-2</v>
       </c>
       <c r="E42" s="36">
         <f>VLOOKUP(C42,Data!$B:$P,4,FALSE)</f>
@@ -21136,7 +21136,7 @@
       </c>
       <c r="D43" s="7">
         <f t="shared" si="11"/>
-        <v>3.3917247428588412E-2</v>
+        <v>3.5994185364379087E-2</v>
       </c>
       <c r="E43" s="36">
         <f>VLOOKUP(C43,Data!$B:$P,4,FALSE)</f>
@@ -21222,7 +21222,7 @@
       </c>
       <c r="D44" s="7">
         <f t="shared" si="11"/>
-        <v>3.3917247428588412E-2</v>
+        <v>3.5994185364379087E-2</v>
       </c>
       <c r="E44" s="36">
         <f>VLOOKUP(C44,Data!$B:$P,4,FALSE)</f>
@@ -21308,7 +21308,7 @@
       </c>
       <c r="D45" s="7">
         <f t="shared" si="11"/>
-        <v>6.2005008889224764E-2</v>
+        <v>6.5801913559694017E-2</v>
       </c>
       <c r="E45" s="36">
         <f>VLOOKUP(C45,Data!$B:$P,4,FALSE)</f>
@@ -21458,7 +21458,7 @@
       <c r="C49" s="6"/>
       <c r="D49" s="43">
         <f>SUM(D31:D48)</f>
-        <v>0.84373963455769574</v>
+        <v>0.89540641142786026</v>
       </c>
       <c r="E49" s="43"/>
       <c r="F49" s="36"/>
@@ -21467,17 +21467,17 @@
       <c r="I49" s="9"/>
       <c r="J49" s="10">
         <f>SUMPRODUCT(J31:J48,D31:D48)</f>
-        <v>4.1479783793291633E-2</v>
+        <v>4.4019817052478441E-2</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="11"/>
       <c r="M49" s="7">
         <f>SUMPRODUCT($D$31:$D$35,M31:M35)</f>
-        <v>9.1581200257227317E-3</v>
+        <v>9.7189216338719655E-3</v>
       </c>
       <c r="N49" s="7">
         <f>SUMPRODUCT($D$31:$D$35,N31:N35)</f>
-        <v>1.9049046563616901E-3</v>
+        <v>2.0215523517028845E-3</v>
       </c>
       <c r="O49" s="36"/>
       <c r="P49" s="40">
@@ -21513,7 +21513,7 @@
       <c r="C50" s="13"/>
       <c r="D50" s="14">
         <f>R50/R51</f>
-        <v>5.7702040336939341E-2</v>
+        <v>0</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="15"/>
@@ -21528,18 +21528,19 @@
       <c r="O50" s="15"/>
       <c r="P50" s="15"/>
       <c r="Q50" s="15">
-        <f>R50*Data!G2/Data!F2</f>
-        <v>11849800</v>
+        <f>SUMIF(Data!$J:$J,"Cash",Data!$G:$G)</f>
+        <v>0</v>
       </c>
       <c r="R50" s="20">
-        <v>200000</v>
+        <f>SUMIF(Data!$J:$J,"Cash",Data!$F:$F)</f>
+        <v>0</v>
       </c>
       <c r="S50" s="21"/>
       <c r="T50" s="22"/>
       <c r="U50" s="18"/>
       <c r="V50" s="20">
         <f>R50</f>
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="W50" s="18"/>
       <c r="X50" s="18"/>
@@ -21561,11 +21562,11 @@
       <c r="L51" s="26"/>
       <c r="M51" s="28">
         <f>M29+M49</f>
-        <v>1.3594896707922306E-2</v>
+        <v>1.4427386336253409E-2</v>
       </c>
       <c r="N51" s="28">
         <f>N29+N49</f>
-        <v>4.832220051527559E-3</v>
+        <v>5.1281232246915042E-3</v>
       </c>
       <c r="O51" s="29">
         <f>SUM(O6:O50)</f>
@@ -21577,11 +21578,11 @@
       </c>
       <c r="Q51" s="29">
         <f>Q29+Q49+Q50</f>
-        <v>205361888.95237499</v>
+        <v>193512088.95237499</v>
       </c>
       <c r="R51" s="29">
         <f>R29+R49+R50</f>
-        <v>3466081.9415074517</v>
+        <v>3266081.9415074517</v>
       </c>
       <c r="S51" s="29">
         <f>S29+S49+S50</f>
@@ -21593,11 +21594,11 @@
       </c>
       <c r="U51" s="28">
         <f>SUMPRODUCT($D$6:$D$48,U6:U48)/100</f>
-        <v>4.8835612379798075E-2</v>
+        <v>5.1826083118401672E-2</v>
       </c>
       <c r="V51" s="29">
         <f>V29+V49+V50</f>
-        <v>3505312.255514896</v>
+        <v>3305312.255514896</v>
       </c>
       <c r="W51" s="28"/>
       <c r="X51" s="28"/>
@@ -25933,7 +25934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1527" workbookViewId="0">
+    <sheetView topLeftCell="A1527" workbookViewId="0">
       <selection activeCell="D1554" sqref="D1554"/>
     </sheetView>
   </sheetViews>

</xml_diff>